<commit_message>
Changed dates to ISO
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AE624C-E952-402C-8BFA-BDAB8ECFFC53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FD379FC-5575-432C-9E88-303148BFE824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="6810" windowWidth="17640" windowHeight="13005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7170" yWindow="2445" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -123,6 +123,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,7 +157,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,12 +441,12 @@
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated population of Geneva
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6A74D7-AC2D-40FF-9532-DF0008D33609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E5963-7ED8-47C8-8CD3-0C51357E87A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19050" yWindow="2835" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2355" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1401,7 @@
         <v>24</v>
       </c>
       <c r="B7">
-        <v>49948</v>
+        <v>495249</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed data source for demography
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E5963-7ED8-47C8-8CD3-0C51357E87A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE54AB84-2DE8-49F2-A0C4-18D7D295D44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2355" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="3135" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,7 +1481,7 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>17685</v>
+        <v>177964</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added partial data for 15. and 16. March
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363FCF3B-183F-40E8-9C5B-B57B5D3058D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F41FDB8-959D-4344-A680-F2D80428C604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="2715" windowWidth="17910" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="1185" windowWidth="24765" windowHeight="16905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
-    <sheet name="demographics" sheetId="3" r:id="rId2"/>
+    <sheet name="Quellen" sheetId="4" r:id="rId2"/>
+    <sheet name="demographics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>ZH</t>
   </si>
@@ -139,6 +140,33 @@
   </si>
   <si>
     <t>BedsPerCapita</t>
+  </si>
+  <si>
+    <t>Quellen:</t>
+  </si>
+  <si>
+    <t>https://www.nw.ch/gesundheitsamtdienste/6044#Anzahl%C2%A0Erkrankungen</t>
+  </si>
+  <si>
+    <t>https://www.besondere-lage.sites.be.ch/besondere-lage_sites/de/index/corona/index.html#originRequestUrl=www.be.ch/corona</t>
+  </si>
+  <si>
+    <t>https://www.sg.ch/tools/informationen-coronavirus.html</t>
+  </si>
+  <si>
+    <t>https://www4.ti.ch/area-media/comunicati/dettaglio-comunicato/?NEWS_ID=187475&amp;tx_tichareamedia_comunicazioni[action]=show&amp;tx_tichareamedia_comunicazioni[controller]=Comunicazioni</t>
+  </si>
+  <si>
+    <t>@sarahhu87422283</t>
+  </si>
+  <si>
+    <t>@borisfritscher</t>
+  </si>
+  <si>
+    <t>https://www.ne.ch/autorites/DFS/SCSP/medecin-cantonal/maladies-vaccinations/Pages/Coronavirus.aspx</t>
+  </si>
+  <si>
+    <t>2327‬</t>
   </si>
 </sst>
 </file>
@@ -148,10 +176,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,14 +210,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,15 +504,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -639,7 +684,7 @@
       <c r="AA2">
         <v>24</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="4">
         <f>SUM(B2:AA2)</f>
         <v>207</v>
       </c>
@@ -726,7 +771,7 @@
       <c r="AA3">
         <v>28</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="4">
         <f>SUM(B3:AA3)</f>
         <v>262</v>
       </c>
@@ -813,7 +858,7 @@
       <c r="AA4">
         <v>34</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="4">
         <f>SUM(B4:AA4)</f>
         <v>331</v>
       </c>
@@ -900,7 +945,7 @@
       <c r="AA5">
         <v>36</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="4">
         <f t="shared" ref="AB5:AB10" si="0">SUM(B5:AA5)</f>
         <v>372</v>
       </c>
@@ -987,7 +1032,7 @@
       <c r="AA6">
         <v>45</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="4">
         <f t="shared" si="0"/>
         <v>490</v>
       </c>
@@ -1074,7 +1119,7 @@
       <c r="AA7">
         <v>55</v>
       </c>
-      <c r="AB7">
+      <c r="AB7" s="4">
         <f t="shared" si="0"/>
         <v>638</v>
       </c>
@@ -1161,7 +1206,7 @@
       <c r="AA8">
         <v>91</v>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="4">
         <f t="shared" si="0"/>
         <v>851</v>
       </c>
@@ -1248,7 +1293,7 @@
       <c r="AA9">
         <v>124</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="4">
         <f t="shared" si="0"/>
         <v>1120</v>
       </c>
@@ -1335,10 +1380,92 @@
       <c r="AA10">
         <v>148</v>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="4">
         <f t="shared" si="0"/>
         <v>1353</v>
       </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43905</v>
+      </c>
+      <c r="T11">
+        <v>13</v>
+      </c>
+      <c r="AB11" s="4">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43906</v>
+      </c>
+      <c r="E12">
+        <v>113</v>
+      </c>
+      <c r="G12">
+        <v>144</v>
+      </c>
+      <c r="N12">
+        <v>74</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="Q12">
+        <v>35</v>
+      </c>
+      <c r="U12">
+        <v>17</v>
+      </c>
+      <c r="V12">
+        <v>330</v>
+      </c>
+      <c r="AA12">
+        <v>270</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB13" s="4"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB14" s="4"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB15" s="4"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB16" s="4"/>
+    </row>
+    <row r="17" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB17" s="4"/>
+    </row>
+    <row r="18" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB18" s="4"/>
+    </row>
+    <row r="19" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB19" s="4"/>
+    </row>
+    <row r="20" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB20" s="4"/>
+    </row>
+    <row r="21" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB21" s="4"/>
+    </row>
+    <row r="22" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB22" s="4"/>
+    </row>
+    <row r="23" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB23" s="4"/>
+    </row>
+    <row r="24" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB24" s="4"/>
+    </row>
+    <row r="25" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB25" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U5:U31">
@@ -1350,10 +1477,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="Anzahl%C2%A0Erkrankungen" display="https://www.nw.ch/gesundheitsamtdienste/6044 - Anzahl%C2%A0Erkrankungen" xr:uid="{368D29F9-18D5-4BE0-A82A-697E4A6494B4}"/>
+    <hyperlink ref="B3" r:id="rId2" location="originRequestUrl=www.be.ch/corona" display="https://www.besondere-lage.sites.be.ch/besondere-lage_sites/de/index/corona/index.html - originRequestUrl=www.be.ch/corona" xr:uid="{90EDDEF4-8D35-4060-B482-4742B1F34CD6}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{DB180D48-A82E-4B10-AD07-E966F5F0A4DC}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www4.ti.ch/area-media/comunicati/dettaglio-comunicato/?NEWS_ID=187475&amp;tx_tichareamedia_comunicazioni%5baction%5d=show&amp;tx_tichareamedia_comunicazioni%5bcontroller%5d=Comunicazioni" xr:uid="{54FC1A73-D5EE-4E98-84BC-4D50BF6BF74C}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{2C76560F-6595-4D27-BA3A-8C03A37CFE59}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new data for *yesterday*
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB845BD-181F-45E2-8311-A5F486C77768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0D7885-3E8F-4B80-BF7E-D4741ACFE041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="1185" windowWidth="24765" windowHeight="16905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="3525" windowWidth="17340" windowHeight="16905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>ZH</t>
   </si>
@@ -164,6 +164,21 @@
   </si>
   <si>
     <t>https://www.ne.ch/autorites/DFS/SCSP/medecin-cantonal/maladies-vaccinations/Pages/Coronavirus.aspx</t>
+  </si>
+  <si>
+    <t>https://www.ag.ch/media/kanton_aargau/themen_1/coronavirus_1/200316_Coronavirus_Bundesrats_Entscheide-2.pdf</t>
+  </si>
+  <si>
+    <t>@BachliMeyer</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCEcqzK6vbCuIvxLiJCAMVuA</t>
+  </si>
+  <si>
+    <t>https://www.ur.ch/mmdirektionen/63458</t>
+  </si>
+  <si>
+    <t>https://www.ai.ch/themen/gesundheit-alter-und-soziales/gesundheitsfoerderung-und-praevention/uebertragbare-krankheiten/coronavirus</t>
   </si>
 </sst>
 </file>
@@ -501,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF19" sqref="AF19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,6 +1410,9 @@
       <c r="A12" s="1">
         <v>43906</v>
       </c>
+      <c r="B12">
+        <v>52</v>
+      </c>
       <c r="E12">
         <v>113</v>
       </c>
@@ -1473,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,6 +1553,47 @@
         <v>41</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="Anzahl%C2%A0Erkrankungen" display="https://www.nw.ch/gesundheitsamtdienste/6044 - Anzahl%C2%A0Erkrankungen" xr:uid="{368D29F9-18D5-4BE0-A82A-697E4A6494B4}"/>
@@ -1542,6 +1601,10 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{DB180D48-A82E-4B10-AD07-E966F5F0A4DC}"/>
     <hyperlink ref="B5" r:id="rId4" display="https://www4.ti.ch/area-media/comunicati/dettaglio-comunicato/?NEWS_ID=187475&amp;tx_tichareamedia_comunicazioni%5baction%5d=show&amp;tx_tichareamedia_comunicazioni%5bcontroller%5d=Comunicazioni" xr:uid="{54FC1A73-D5EE-4E98-84BC-4D50BF6BF74C}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{2C76560F-6595-4D27-BA3A-8C03A37CFE59}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{ADDE70E2-B49C-4416-81AF-41854C094A62}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{6C375F2D-514B-4B3B-ABDA-DC5146FA2A02}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{A31E6CF7-91A7-4D97-B47D-3F52557EF47C}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{10400BC4-69C6-43F2-8E09-A52E1A451E9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated AI and UR
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0D7885-3E8F-4B80-BF7E-D4741ACFE041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9694DC6B-8DDE-49D3-9C3B-1018A4D9376A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="3525" windowWidth="17340" windowHeight="16905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1289,7 @@
         <v>218</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X9">
         <v>222</v>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="AB9" s="4">
         <f t="shared" si="0"/>
-        <v>1120</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>31</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1376,7 +1376,7 @@
         <v>262</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X10">
         <v>273</v>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="AB10" s="4">
         <f t="shared" si="0"/>
-        <v>1353</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1493,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated data 17. 03.
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9694DC6B-8DDE-49D3-9C3B-1018A4D9376A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297A9A22-5332-4B3E-8912-16B557380BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15960" yWindow="2745" windowWidth="21075" windowHeight="16905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,7 +1442,18 @@
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="AB13" s="4"/>
+      <c r="A13" s="1">
+        <v>43907</v>
+      </c>
+      <c r="N13">
+        <v>77</v>
+      </c>
+      <c r="AA13">
+        <v>294</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>2650</v>
+      </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB14" s="4"/>
@@ -1494,7 +1505,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Switzerland to demographics
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E1E13E-3129-405A-B9DF-DC980AAAD3DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA7BC08-B27D-40D6-A024-512CCBBC271E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="2025" windowWidth="27480" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="2025" windowWidth="27480" windowHeight="17775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>ZH</t>
   </si>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1644,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,7 +1725,7 @@
         <v>3053</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G27" si="1">F3/B3</f>
+        <f t="shared" ref="G3:G28" si="1">F3/B3</f>
         <v>2.9498240057508522E-3</v>
       </c>
     </row>
@@ -2327,6 +2327,35 @@
       <c r="G27">
         <f t="shared" si="1"/>
         <v>1.1148962527098173E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>SUM(B2:B27)</f>
+        <v>8541410</v>
+      </c>
+      <c r="C28">
+        <f>AVERAGE(C2:C27)</f>
+        <v>495.07692307692309</v>
+      </c>
+      <c r="D28">
+        <f>AVERAGE(D2:D27)</f>
+        <v>0.19099999999999998</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E2:E27)</f>
+        <v>1576463</v>
+      </c>
+      <c r="F28">
+        <f>SUM(F2:F27)</f>
+        <v>23111</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>2.7057593535493554E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TI, AG, and NW
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA7BC08-B27D-40D6-A024-512CCBBC271E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD277FD3-CA99-48B4-96D4-50A4E276F986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="2025" windowWidth="27480" windowHeight="17775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="2040" windowWidth="27480" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,8 +1451,20 @@
       <c r="A13" s="1">
         <v>43907</v>
       </c>
+      <c r="B13">
+        <v>67</v>
+      </c>
       <c r="N13">
         <v>77</v>
+      </c>
+      <c r="O13">
+        <v>12</v>
+      </c>
+      <c r="Q13">
+        <v>47</v>
+      </c>
+      <c r="V13">
+        <v>422</v>
       </c>
       <c r="Y13">
         <v>95</v>
@@ -1514,7 +1526,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated GE, JU, BS
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD277FD3-CA99-48B4-96D4-50A4E276F986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AD682A-DA7E-417E-9894-A9C6C44C2029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="2040" windowWidth="27480" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6555" yWindow="3045" windowWidth="27480" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>ZH</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>@enno_hermann</t>
+  </si>
+  <si>
+    <t>https://www.coronavirus.bs.ch</t>
+  </si>
+  <si>
+    <t>https://www.jura.ch/fr/Autorites/Coronavirus/Accueil/Coronavirus-Informations-officielles-a-la-population-jurassienne.html</t>
+  </si>
+  <si>
+    <t>https://www.ge.ch/document/point-coronavirus-maladie-covid-19</t>
   </si>
 </sst>
 </file>
@@ -523,7 +532,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,6 +1414,9 @@
       <c r="A11" s="1">
         <v>43905</v>
       </c>
+      <c r="I11">
+        <v>294</v>
+      </c>
       <c r="T11">
         <v>13</v>
       </c>
@@ -1425,6 +1437,9 @@
       <c r="G12">
         <v>144</v>
       </c>
+      <c r="I12">
+        <v>382</v>
+      </c>
       <c r="N12">
         <v>74</v>
       </c>
@@ -1453,6 +1468,12 @@
       </c>
       <c r="B13">
         <v>67</v>
+      </c>
+      <c r="G13">
+        <v>165</v>
+      </c>
+      <c r="L13">
+        <v>23</v>
       </c>
       <c r="N13">
         <v>77</v>
@@ -1523,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,6 +1656,30 @@
       </c>
       <c r="C11" s="3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1649,6 +1694,9 @@
     <hyperlink ref="B10" r:id="rId8" xr:uid="{A31E6CF7-91A7-4D97-B47D-3F52557EF47C}"/>
     <hyperlink ref="B9" r:id="rId9" xr:uid="{10400BC4-69C6-43F2-8E09-A52E1A451E9C}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{30961DFB-4E45-4611-A82F-A2689E420CC1}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{07F612FA-0C2F-4064-82BD-F93037B19CD8}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added LU and VD
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AD682A-DA7E-417E-9894-A9C6C44C2029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF55E7A6-0AF6-483C-A9AB-53AF3B7D4D58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="3045" windowWidth="27480" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="1410" windowWidth="27480" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>ZH</t>
   </si>
@@ -194,6 +194,24 @@
   </si>
   <si>
     <t>https://www.ge.ch/document/point-coronavirus-maladie-covid-19</t>
+  </si>
+  <si>
+    <t>https://www.luzernerzeitung.ch/zentralschweiz/luzern/so-will-die-luzerner-regierung-die-massnahmen-des-bundes-umsetzen-lukb-stellt-50-millionen-franken-bereit-ld.1204954</t>
+  </si>
+  <si>
+    <t>@neph_b</t>
+  </si>
+  <si>
+    <t>* Official statement in video</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>https://www.24heures.ch/vaud-regions/Les-contaminations-sont-en-hausse-dans-le-canton-de-Vaud/story/23084946?cache=9efAwefu</t>
+  </si>
+  <si>
+    <t>@f_giroud</t>
   </si>
 </sst>
 </file>
@@ -532,7 +550,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,6 +1438,9 @@
       <c r="T11">
         <v>13</v>
       </c>
+      <c r="X11">
+        <v>331</v>
+      </c>
       <c r="AB11" s="4">
         <v>2155</v>
       </c>
@@ -1432,7 +1453,7 @@
         <v>52</v>
       </c>
       <c r="E12">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="G12">
         <v>144</v>
@@ -1454,6 +1475,9 @@
       </c>
       <c r="V12">
         <v>330</v>
+      </c>
+      <c r="X12">
+        <v>461</v>
       </c>
       <c r="AA12">
         <v>270</v>
@@ -1475,6 +1499,9 @@
       <c r="L13">
         <v>23</v>
       </c>
+      <c r="M13">
+        <v>50</v>
+      </c>
       <c r="N13">
         <v>77</v>
       </c>
@@ -1486,6 +1513,9 @@
       </c>
       <c r="V13">
         <v>422</v>
+      </c>
+      <c r="X13">
+        <v>695</v>
       </c>
       <c r="Y13">
         <v>95</v>
@@ -1544,23 +1574,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="180.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1568,7 +1599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1576,7 +1607,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1584,7 +1615,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1595,7 +1626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1606,7 +1637,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1617,7 +1648,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1625,7 +1656,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1667,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +1678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1658,7 +1689,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1666,7 +1697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1674,12 +1705,37 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1697,14 +1753,17 @@
     <hyperlink ref="B12" r:id="rId11" xr:uid="{07F612FA-0C2F-4064-82BD-F93037B19CD8}"/>
     <hyperlink ref="B13" r:id="rId12" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
     <hyperlink ref="B14" r:id="rId13" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
@@ -2114,7 +2173,7 @@
         <v>6.1561052750480063E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2139,7 +2198,7 @@
         <v>2.1633588815715538E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2164,7 +2223,7 @@
         <v>1.7214839945968021E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2189,7 +2248,7 @@
         <v>1.6241317596600361E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2214,7 +2273,7 @@
         <v>2.2685416692075958E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2239,7 +2298,7 @@
         <v>1.9749656083575097E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2264,7 +2323,7 @@
         <v>3.7657964297353082E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2289,7 +2348,7 @@
         <v>1.6889156236263101E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2313,8 +2372,11 @@
         <f t="shared" si="1"/>
         <v>2.1285548102863649E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2339,7 +2401,7 @@
         <v>1.3213181469834306E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2364,7 +2426,7 @@
         <v>1.7292015480471002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2389,7 +2451,7 @@
         <v>1.1148962527098173E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Added update for BE,BS,NW,TG,ZH,NE,SG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF55E7A6-0AF6-483C-A9AB-53AF3B7D4D58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8EFB61-4010-4767-9041-D62F61EB9A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="1410" windowWidth="27480" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="2325" windowWidth="19200" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
-    <sheet name="Quellen" sheetId="4" r:id="rId2"/>
-    <sheet name="demographics" sheetId="3" r:id="rId3"/>
+    <sheet name="Tests" sheetId="5" r:id="rId2"/>
+    <sheet name="Quellen" sheetId="4" r:id="rId3"/>
+    <sheet name="demographics" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
   <si>
     <t>ZH</t>
   </si>
@@ -212,6 +213,9 @@
   </si>
   <si>
     <t>@f_giroud</t>
+  </si>
+  <si>
+    <t>https://www.tg.ch/news/fachdossier-coronavirus.html/10552</t>
   </si>
 </sst>
 </file>
@@ -550,7 +554,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,6 +1515,9 @@
       <c r="Q13">
         <v>47</v>
       </c>
+      <c r="U13">
+        <v>23</v>
+      </c>
       <c r="V13">
         <v>422</v>
       </c>
@@ -1528,6 +1535,30 @@
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43908</v>
+      </c>
+      <c r="E14">
+        <v>193</v>
+      </c>
+      <c r="G14">
+        <v>182</v>
+      </c>
+      <c r="N14">
+        <v>99</v>
+      </c>
+      <c r="O14">
+        <v>12</v>
+      </c>
+      <c r="Q14">
+        <v>61</v>
+      </c>
+      <c r="U14">
+        <v>32</v>
+      </c>
+      <c r="AA14">
+        <v>424</v>
+      </c>
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -1573,11 +1604,191 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB15D9C-377E-4F66-998B-5427F83AE200}">
+  <dimension ref="A1:AB13"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43896</v>
+      </c>
+      <c r="AB2" s="4"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43897</v>
+      </c>
+      <c r="AB3" s="4"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43898</v>
+      </c>
+      <c r="AB4" s="4"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43899</v>
+      </c>
+      <c r="AB5" s="4"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43900</v>
+      </c>
+      <c r="AB6" s="4"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43901</v>
+      </c>
+      <c r="AB7" s="4"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43902</v>
+      </c>
+      <c r="AB8" s="4"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43903</v>
+      </c>
+      <c r="AB9" s="4"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43904</v>
+      </c>
+      <c r="AB10" s="4"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43905</v>
+      </c>
+      <c r="AB11" s="4"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43906</v>
+      </c>
+      <c r="AB12" s="5"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43907</v>
+      </c>
+      <c r="U13">
+        <v>276</v>
+      </c>
+      <c r="AB13" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,10 +1949,18 @@
         <v>58</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="Anzahl%C2%A0Erkrankungen" display="https://www.nw.ch/gesundheitsamtdienste/6044 - Anzahl%C2%A0Erkrankungen" xr:uid="{368D29F9-18D5-4BE0-A82A-697E4A6494B4}"/>
-    <hyperlink ref="B3" r:id="rId2" location="originRequestUrl=www.be.ch/corona" display="https://www.besondere-lage.sites.be.ch/besondere-lage_sites/de/index/corona/index.html - originRequestUrl=www.be.ch/corona" xr:uid="{90EDDEF4-8D35-4060-B482-4742B1F34CD6}"/>
+    <hyperlink ref="B3" r:id="rId2" location="originRequestUrl=www.be.ch/corona" xr:uid="{90EDDEF4-8D35-4060-B482-4742B1F34CD6}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{DB180D48-A82E-4B10-AD07-E966F5F0A4DC}"/>
     <hyperlink ref="B5" r:id="rId4" display="https://www4.ti.ch/area-media/comunicati/dettaglio-comunicato/?NEWS_ID=187475&amp;tx_tichareamedia_comunicazioni%5baction%5d=show&amp;tx_tichareamedia_comunicazioni%5bcontroller%5d=Comunicazioni" xr:uid="{54FC1A73-D5EE-4E98-84BC-4D50BF6BF74C}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{2C76560F-6595-4D27-BA3A-8C03A37CFE59}"/>
@@ -1755,13 +1974,14 @@
     <hyperlink ref="B14" r:id="rId13" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
     <hyperlink ref="B15" r:id="rId14" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
     <hyperlink ref="B16" r:id="rId15" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
   <dimension ref="A1:M28"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated BL and SH
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8EFB61-4010-4767-9041-D62F61EB9A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D816153E-48EC-4530-A1A1-FB33A13D64A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="2325" windowWidth="19200" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1890" windowWidth="23430" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
   <si>
     <t>ZH</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>https://www.tg.ch/news/fachdossier-coronavirus.html/10552</t>
+  </si>
+  <si>
+    <t>https://sh.ch/CMS/Webseite/Kanton-Schaffhausen/Beh-rde/Verwaltung/Departement-des-Innern/Gesundheitsamt-3209198-DE.html</t>
+  </si>
+  <si>
+    <t>https://www.baselland.ch/</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,6 +1547,9 @@
       <c r="E14">
         <v>193</v>
       </c>
+      <c r="F14">
+        <v>116</v>
+      </c>
       <c r="G14">
         <v>182</v>
       </c>
@@ -1552,6 +1561,9 @@
       </c>
       <c r="Q14">
         <v>61</v>
+      </c>
+      <c r="R14">
+        <v>6</v>
       </c>
       <c r="U14">
         <v>32</v>
@@ -1785,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,12 +1961,34 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1975,9 +2009,11 @@
     <hyperlink ref="B15" r:id="rId14" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
     <hyperlink ref="B16" r:id="rId15" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
     <hyperlink ref="B17" r:id="rId16" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated data from BAG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D816153E-48EC-4530-A1A1-FB33A13D64A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8060A61D-796F-4A11-84BF-5B30CF773D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1890" windowWidth="23430" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="2475" windowWidth="18600" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="61">
   <si>
     <t>ZH</t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>* Official statement in video</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>https://www.24heures.ch/vaud-regions/Les-contaminations-sont-en-hausse-dans-le-canton-de-Vaud/story/23084946?cache=9efAwefu</t>
@@ -560,7 +557,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,6 +1541,15 @@
       <c r="A14" s="1">
         <v>43908</v>
       </c>
+      <c r="B14">
+        <v>69</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
       <c r="E14">
         <v>193</v>
       </c>
@@ -1551,7 +1557,19 @@
         <v>116</v>
       </c>
       <c r="G14">
-        <v>182</v>
+        <v>207</v>
+      </c>
+      <c r="H14">
+        <v>67</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>95</v>
+      </c>
+      <c r="M14">
+        <v>48</v>
       </c>
       <c r="N14">
         <v>99</v>
@@ -1559,19 +1577,42 @@
       <c r="O14">
         <v>12</v>
       </c>
+      <c r="P14">
+        <v>16</v>
+      </c>
       <c r="Q14">
         <v>61</v>
       </c>
       <c r="R14">
         <v>6</v>
       </c>
+      <c r="S14">
+        <v>31</v>
+      </c>
+      <c r="T14">
+        <v>29</v>
+      </c>
       <c r="U14">
         <v>32</v>
       </c>
+      <c r="V14">
+        <v>506</v>
+      </c>
+      <c r="X14">
+        <v>721</v>
+      </c>
+      <c r="Y14">
+        <v>129</v>
+      </c>
+      <c r="Z14">
+        <v>17</v>
+      </c>
       <c r="AA14">
         <v>424</v>
       </c>
-      <c r="AB14" s="4"/>
+      <c r="AB14" s="4">
+        <v>3028</v>
+      </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB15" s="4"/>
@@ -1955,10 +1996,10 @@
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,7 +2007,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1974,7 +2015,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>44</v>
@@ -1985,7 +2026,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>44</v>
@@ -2019,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="O27" sqref="N2:O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,7 +2072,7 @@
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2054,7 +2095,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2078,8 +2119,22 @@
         <f>F2/B2</f>
         <v>2.9402327991121442E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>B2/100000</f>
+        <v>15.209680000000001</v>
+      </c>
+      <c r="M2">
+        <v>21.8</v>
+      </c>
+      <c r="N2">
+        <f>ROUND(L2*M2,0)</f>
+        <v>332</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2103,8 +2158,22 @@
         <f t="shared" ref="G3:G28" si="1">F3/B3</f>
         <v>2.9498240057508522E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L28" si="2">B3/100000</f>
+        <v>10.349769999999999</v>
+      </c>
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N28" si="3">ROUND(L3*M3,0)</f>
+        <v>155</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2128,8 +2197,22 @@
         <f t="shared" si="1"/>
         <v>2.8380331479268468E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>7.9914500000000004</v>
+      </c>
+      <c r="M4">
+        <v>90.2</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="3"/>
+        <v>721</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2153,8 +2236,22 @@
         <f t="shared" si="1"/>
         <v>2.1379903185900469E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>6.78207</v>
+      </c>
+      <c r="M5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="O5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2178,8 +2275,22 @@
         <f t="shared" si="1"/>
         <v>3.0825472673661654E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>5.0769700000000002</v>
+      </c>
+      <c r="M6">
+        <v>12.2</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2203,8 +2314,22 @@
         <f t="shared" si="1"/>
         <v>3.0408945803020301E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>4.9524900000000001</v>
+      </c>
+      <c r="M7">
+        <v>50.7</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2228,8 +2353,22 @@
         <f t="shared" si="1"/>
         <v>2.3855043376135678E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>4.0955700000000004</v>
+      </c>
+      <c r="M8">
+        <v>11.7</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="O8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2253,8 +2392,22 @@
         <f t="shared" si="1"/>
         <v>3.7866888547388798E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>3.5334300000000001</v>
+      </c>
+      <c r="M9">
+        <v>143.19999999999999</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>506</v>
+      </c>
+      <c r="O9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2278,8 +2431,22 @@
         <f t="shared" si="1"/>
         <v>2.4247357939265312E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>3.4395500000000001</v>
+      </c>
+      <c r="M10">
+        <v>37.5</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+      <c r="O10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2303,8 +2470,22 @@
         <f t="shared" si="1"/>
         <v>1.7162722691817743E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>3.1871399999999999</v>
+      </c>
+      <c r="M11">
+        <v>21</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="O11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2328,8 +2509,22 @@
         <f t="shared" si="1"/>
         <v>2.0199075423764108E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>2.8813200000000001</v>
+      </c>
+      <c r="M12">
+        <v>39.6</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="O12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2353,8 +2548,22 @@
         <f t="shared" si="1"/>
         <v>2.0616915998726815E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>2.7647200000000001</v>
+      </c>
+      <c r="M13">
+        <v>6.9</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="O13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2378,8 +2587,22 @@
         <f t="shared" si="1"/>
         <v>1.8668052739079189E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>2.7319399999999998</v>
+      </c>
+      <c r="M14">
+        <v>11.3</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="O14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2403,8 +2626,22 @@
         <f t="shared" si="1"/>
         <v>2.7523074518976303E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>1.9837899999999999</v>
+      </c>
+      <c r="M15">
+        <v>47.9</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="O15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2428,8 +2665,22 @@
         <f t="shared" si="1"/>
         <v>6.1561052750480063E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>1.9476599999999999</v>
+      </c>
+      <c r="M16">
+        <v>106.3</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+      <c r="O16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2453,8 +2704,22 @@
         <f t="shared" si="1"/>
         <v>2.1633588815715538E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>1.7796400000000001</v>
+      </c>
+      <c r="M17">
+        <v>43</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="O17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2478,8 +2743,22 @@
         <f t="shared" si="1"/>
         <v>1.7214839945968021E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>1.59165</v>
+      </c>
+      <c r="M18">
+        <v>18.2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="O18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2503,8 +2782,22 @@
         <f t="shared" si="1"/>
         <v>1.6241317596600361E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>1.26837</v>
+      </c>
+      <c r="M19">
+        <v>13.4</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="O19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2528,8 +2821,22 @@
         <f t="shared" si="1"/>
         <v>2.2685416692075958E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>0.81991000000000003</v>
+      </c>
+      <c r="M20">
+        <v>2.4</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="O20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2553,8 +2860,22 @@
         <f t="shared" si="1"/>
         <v>1.9749656083575097E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>0.73419000000000001</v>
+      </c>
+      <c r="M21">
+        <v>30</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="O21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2578,8 +2899,22 @@
         <f t="shared" si="1"/>
         <v>3.7657964297353082E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>0.55234000000000005</v>
+      </c>
+      <c r="M22">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="O22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2603,8 +2938,22 @@
         <f t="shared" si="1"/>
         <v>1.6889156236263101E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>0.43223</v>
+      </c>
+      <c r="M23">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="O23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2628,11 +2977,22 @@
         <f t="shared" si="1"/>
         <v>2.1285548102863649E-3</v>
       </c>
-      <c r="M24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>0.40403</v>
+      </c>
+      <c r="M24">
+        <v>24.8</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="O24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2656,8 +3016,22 @@
         <f t="shared" si="1"/>
         <v>1.3213181469834306E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>0.37841000000000002</v>
+      </c>
+      <c r="M25">
+        <v>42.3</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="O25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2681,8 +3055,22 @@
         <f t="shared" si="1"/>
         <v>1.7292015480471002E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>0.36432999999999999</v>
+      </c>
+      <c r="M26">
+        <v>2.7</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2706,8 +3094,22 @@
         <f t="shared" si="1"/>
         <v>1.1148962527098173E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>0.16145000000000001</v>
+      </c>
+      <c r="M27">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="O27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2734,6 +3136,17 @@
       <c r="G28">
         <f t="shared" si="1"/>
         <v>2.7057593535493554E-3</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>85.414100000000005</v>
+      </c>
+      <c r="N28">
+        <f>SUM(N2:N27)</f>
+        <v>3008</v>
+      </c>
+      <c r="O28" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AG, BS and UR
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8060A61D-796F-4A11-84BF-5B30CF773D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F5BDA0-6BE7-4F03-A778-AA998E857A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2145" yWindow="2475" windowWidth="18600" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="62">
   <si>
     <t>ZH</t>
   </si>
@@ -167,9 +167,6 @@
     <t>https://www.ne.ch/autorites/DFS/SCSP/medecin-cantonal/maladies-vaccinations/Pages/Coronavirus.aspx</t>
   </si>
   <si>
-    <t>https://www.ag.ch/media/kanton_aargau/themen_1/coronavirus_1/200316_Coronavirus_Bundesrats_Entscheide-2.pdf</t>
-  </si>
-  <si>
     <t>@BachliMeyer</t>
   </si>
   <si>
@@ -219,6 +216,12 @@
   </si>
   <si>
     <t>https://www.baselland.ch/</t>
+  </si>
+  <si>
+    <t>https://www.ag.ch/de/themen_1/coronavirus_2/coronavirus.jsp</t>
+  </si>
+  <si>
+    <t>https://www.coronavirus.bs.ch/</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1545,7 @@
         <v>43908</v>
       </c>
       <c r="B14">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -1557,7 +1560,7 @@
         <v>116</v>
       </c>
       <c r="G14">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="H14">
         <v>67</v>
@@ -1568,6 +1571,9 @@
       <c r="K14">
         <v>95</v>
       </c>
+      <c r="L14">
+        <v>25</v>
+      </c>
       <c r="M14">
         <v>48</v>
       </c>
@@ -1596,7 +1602,10 @@
         <v>32</v>
       </c>
       <c r="V14">
-        <v>506</v>
+        <v>511</v>
+      </c>
+      <c r="W14">
+        <v>5</v>
       </c>
       <c r="X14">
         <v>721</v>
@@ -1838,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,10 +1915,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1917,7 +1926,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,10 +1934,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1936,10 +1945,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,10 +1956,10 @@
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1958,7 +1967,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,7 +1975,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1974,7 +1983,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1982,13 +1991,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1996,10 +2005,10 @@
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2007,7 +2016,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2015,10 +2024,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,10 +2035,18 @@
         <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2052,9 +2069,10 @@
     <hyperlink ref="B17" r:id="rId16" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
     <hyperlink ref="B18" r:id="rId17" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
     <hyperlink ref="B19" r:id="rId18" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -2166,7 +2184,7 @@
         <v>15</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N28" si="3">ROUND(L3*M3,0)</f>
+        <f t="shared" ref="N3:N27" si="3">ROUND(L3*M3,0)</f>
         <v>155</v>
       </c>
       <c r="O3" t="s">

</xml_diff>

<commit_message>
Updated GR, TG, SG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F5BDA0-6BE7-4F03-A778-AA998E857A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB7AE49-7FFA-47BA-AD3F-234F97360E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2475" windowWidth="18600" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="2220" windowWidth="18600" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
-    <sheet name="Tests" sheetId="5" r:id="rId2"/>
-    <sheet name="Quellen" sheetId="4" r:id="rId3"/>
+    <sheet name="Quellen" sheetId="4" r:id="rId2"/>
+    <sheet name="Tests" sheetId="5" r:id="rId3"/>
     <sheet name="demographics" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -170,9 +170,6 @@
     <t>@BachliMeyer</t>
   </si>
   <si>
-    <t>https://www.youtube.com/channel/UCEcqzK6vbCuIvxLiJCAMVuA</t>
-  </si>
-  <si>
     <t>https://www.ur.ch/mmdirektionen/63458</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>https://www.coronavirus.bs.ch/</t>
+  </si>
+  <si>
+    <t>https://www.gr.ch/DE/institutionen/verwaltung/djsg/ga/coronavirus/info/Seiten/Start.aspx</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,11 +1565,14 @@
       <c r="H14">
         <v>67</v>
       </c>
+      <c r="I14">
+        <v>468</v>
+      </c>
       <c r="J14">
         <v>10</v>
       </c>
       <c r="K14">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="L14">
         <v>25</v>
@@ -1581,7 +1584,7 @@
         <v>99</v>
       </c>
       <c r="O14">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="P14">
         <v>16</v>
@@ -1624,6 +1627,15 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43909</v>
+      </c>
+      <c r="Q15">
+        <v>85</v>
+      </c>
+      <c r="U15">
+        <v>36</v>
+      </c>
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -1666,11 +1678,242 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="180.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="Anzahl%C2%A0Erkrankungen" display="https://www.nw.ch/gesundheitsamtdienste/6044 - Anzahl%C2%A0Erkrankungen" xr:uid="{368D29F9-18D5-4BE0-A82A-697E4A6494B4}"/>
+    <hyperlink ref="B3" r:id="rId2" location="originRequestUrl=www.be.ch/corona" xr:uid="{90EDDEF4-8D35-4060-B482-4742B1F34CD6}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{DB180D48-A82E-4B10-AD07-E966F5F0A4DC}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www4.ti.ch/area-media/comunicati/dettaglio-comunicato/?NEWS_ID=187475&amp;tx_tichareamedia_comunicazioni%5baction%5d=show&amp;tx_tichareamedia_comunicazioni%5bcontroller%5d=Comunicazioni" xr:uid="{54FC1A73-D5EE-4E98-84BC-4D50BF6BF74C}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{2C76560F-6595-4D27-BA3A-8C03A37CFE59}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{ADDE70E2-B49C-4416-81AF-41854C094A62}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{A31E6CF7-91A7-4D97-B47D-3F52557EF47C}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{10400BC4-69C6-43F2-8E09-A52E1A451E9C}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{30961DFB-4E45-4611-A82F-A2689E420CC1}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{07F612FA-0C2F-4064-82BD-F93037B19CD8}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
+    <hyperlink ref="B8" r:id="rId19" xr:uid="{31E99BB6-82A4-4C45-B793-5F63A7878891}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB15D9C-377E-4F66-998B-5427F83AE200}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,237 +2085,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="180.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="Anzahl%C2%A0Erkrankungen" display="https://www.nw.ch/gesundheitsamtdienste/6044 - Anzahl%C2%A0Erkrankungen" xr:uid="{368D29F9-18D5-4BE0-A82A-697E4A6494B4}"/>
-    <hyperlink ref="B3" r:id="rId2" location="originRequestUrl=www.be.ch/corona" xr:uid="{90EDDEF4-8D35-4060-B482-4742B1F34CD6}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{DB180D48-A82E-4B10-AD07-E966F5F0A4DC}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://www4.ti.ch/area-media/comunicati/dettaglio-comunicato/?NEWS_ID=187475&amp;tx_tichareamedia_comunicazioni%5baction%5d=show&amp;tx_tichareamedia_comunicazioni%5bcontroller%5d=Comunicazioni" xr:uid="{54FC1A73-D5EE-4E98-84BC-4D50BF6BF74C}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{2C76560F-6595-4D27-BA3A-8C03A37CFE59}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{ADDE70E2-B49C-4416-81AF-41854C094A62}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{6C375F2D-514B-4B3B-ABDA-DC5146FA2A02}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{A31E6CF7-91A7-4D97-B47D-3F52557EF47C}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{10400BC4-69C6-43F2-8E09-A52E1A451E9C}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{30961DFB-4E45-4611-A82F-A2689E420CC1}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{07F612FA-0C2F-4064-82BD-F93037B19CD8}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated from BAG incidence numbers
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A1CEDD-59F8-42DB-8326-43A3369768B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C841D0-8D16-4D5C-A09B-9E0BAD2E889E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="2220" windowWidth="18600" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="63">
   <si>
     <t>ZH</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>https://www4.ti.ch/area-media/comunicati/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">: </t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,22 +1633,75 @@
       <c r="A15" s="1">
         <v>43909</v>
       </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>215</v>
+      </c>
+      <c r="F15">
+        <v>139</v>
+      </c>
       <c r="G15">
         <v>222</v>
       </c>
+      <c r="H15">
+        <v>82</v>
+      </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>123</v>
+      </c>
+      <c r="L15">
+        <v>25</v>
+      </c>
+      <c r="M15">
+        <v>63</v>
+      </c>
+      <c r="O15">
+        <v>20</v>
+      </c>
+      <c r="P15">
+        <v>17</v>
+      </c>
       <c r="Q15">
         <v>85</v>
       </c>
+      <c r="R15">
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <v>39</v>
+      </c>
+      <c r="T15">
+        <v>35</v>
+      </c>
       <c r="U15">
         <v>36</v>
       </c>
       <c r="V15">
         <v>638</v>
       </c>
+      <c r="X15">
+        <v>919</v>
+      </c>
+      <c r="Y15">
+        <v>176</v>
+      </c>
+      <c r="Z15">
+        <v>23</v>
+      </c>
       <c r="AA15">
         <v>526</v>
       </c>
-      <c r="AB15" s="4"/>
+      <c r="AB15">
+        <v>3855</v>
+      </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="AB16" s="4"/>
@@ -2099,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O27" sqref="N2:O27"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q28" sqref="O2:Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,7 +2167,7 @@
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2134,7 +2190,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2163,17 +2219,20 @@
         <v>15.209680000000001</v>
       </c>
       <c r="M2">
-        <v>21.8</v>
-      </c>
-      <c r="N2">
+        <v>30.1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2">
         <f>ROUND(L2*M2,0)</f>
-        <v>332</v>
-      </c>
-      <c r="O2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2202,17 +2261,20 @@
         <v>10.349769999999999</v>
       </c>
       <c r="M3">
-        <v>15</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N27" si="3">ROUND(L3*M3,0)</f>
-        <v>155</v>
+        <v>20.8</v>
       </c>
       <c r="O3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3">
+        <f>ROUND(L3*M3,0)</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2241,17 +2303,20 @@
         <v>7.9914500000000004</v>
       </c>
       <c r="M4">
-        <v>90.2</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="3"/>
-        <v>721</v>
+        <v>115</v>
       </c>
       <c r="O4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q4">
+        <f>ROUND(L4*M4,0)</f>
+        <v>919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2280,17 +2345,20 @@
         <v>6.78207</v>
       </c>
       <c r="M5">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="3"/>
-        <v>69</v>
+        <v>14.2</v>
       </c>
       <c r="O5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5">
+        <f>ROUND(L5*M5,0)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2319,17 +2387,20 @@
         <v>5.0769700000000002</v>
       </c>
       <c r="M6">
-        <v>12.2</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="3"/>
-        <v>62</v>
+        <v>17.3</v>
       </c>
       <c r="O6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6">
+        <f>ROUND(L6*M6,0)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2358,17 +2429,20 @@
         <v>4.9524900000000001</v>
       </c>
       <c r="M7">
-        <v>50.7</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="3"/>
-        <v>251</v>
+        <v>61.9</v>
       </c>
       <c r="O7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7">
+        <f>ROUND(L7*M7,0)</f>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2397,17 +2471,20 @@
         <v>4.0955700000000004</v>
       </c>
       <c r="M8">
-        <v>11.7</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="3"/>
-        <v>48</v>
+        <v>15.4</v>
       </c>
       <c r="O8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q8">
+        <f>ROUND(L8*M8,0)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2436,17 +2513,20 @@
         <v>3.5334300000000001</v>
       </c>
       <c r="M9">
-        <v>143.19999999999999</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="3"/>
-        <v>506</v>
+        <v>178.6</v>
       </c>
       <c r="O9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q9">
+        <f>ROUND(L9*M9,0)</f>
+        <v>631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2475,17 +2555,20 @@
         <v>3.4395500000000001</v>
       </c>
       <c r="M10">
-        <v>37.5</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="3"/>
-        <v>129</v>
+        <v>51.2</v>
       </c>
       <c r="O10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q10">
+        <f>ROUND(L10*M10,0)</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2514,17 +2597,20 @@
         <v>3.1871399999999999</v>
       </c>
       <c r="M11">
-        <v>21</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="3"/>
-        <v>67</v>
+        <v>25.7</v>
       </c>
       <c r="O11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q11">
+        <f>ROUND(L11*M11,0)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2553,17 +2639,20 @@
         <v>2.8813200000000001</v>
       </c>
       <c r="M12">
-        <v>39.6</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="3"/>
-        <v>114</v>
+        <v>48.2</v>
       </c>
       <c r="O12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q12">
+        <f>ROUND(L12*M12,0)</f>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2592,17 +2681,20 @@
         <v>2.7647200000000001</v>
       </c>
       <c r="M13">
-        <v>6.9</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="3"/>
-        <v>19</v>
+        <v>10.1</v>
       </c>
       <c r="O13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q13">
+        <f>ROUND(L13*M13,0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2631,17 +2723,20 @@
         <v>2.7319399999999998</v>
       </c>
       <c r="M14">
-        <v>11.3</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="3"/>
-        <v>31</v>
+        <v>14.3</v>
       </c>
       <c r="O14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q14">
+        <f>ROUND(L14*M14,0)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2670,17 +2765,20 @@
         <v>1.9837899999999999</v>
       </c>
       <c r="M15">
-        <v>47.9</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="3"/>
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="O15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q15">
+        <f>ROUND(L15*M15,0)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2709,17 +2807,20 @@
         <v>1.9476599999999999</v>
       </c>
       <c r="M16">
-        <v>106.3</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="3"/>
-        <v>207</v>
+        <v>122.7</v>
       </c>
       <c r="O16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q16">
+        <f>ROUND(L16*M16,0)</f>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2748,17 +2849,20 @@
         <v>1.7796400000000001</v>
       </c>
       <c r="M17">
-        <v>43</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="3"/>
-        <v>77</v>
+        <v>49.2</v>
       </c>
       <c r="O17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17">
+        <f>ROUND(L17*M17,0)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2787,17 +2891,20 @@
         <v>1.59165</v>
       </c>
       <c r="M18">
-        <v>18.2</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="O18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18">
+        <f>ROUND(L18*M18,0)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2826,17 +2933,20 @@
         <v>1.26837</v>
       </c>
       <c r="M19">
-        <v>13.4</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="O19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19">
+        <f>ROUND(L19*M19,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2865,17 +2975,20 @@
         <v>0.81991000000000003</v>
       </c>
       <c r="M20">
-        <v>2.4</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="O20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q20">
+        <f>ROUND(L20*M20,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2904,17 +3017,20 @@
         <v>0.73419000000000001</v>
       </c>
       <c r="M21">
-        <v>30</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="3"/>
-        <v>22</v>
+        <v>34.1</v>
       </c>
       <c r="O21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q21">
+        <f>ROUND(L21*M21,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2943,17 +3059,20 @@
         <v>0.55234000000000005</v>
       </c>
       <c r="M22">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="3"/>
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="O22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q22">
+        <f>ROUND(L22*M22,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2982,17 +3101,20 @@
         <v>0.43223</v>
       </c>
       <c r="M23">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>46.3</v>
       </c>
       <c r="O23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q23">
+        <f>ROUND(L23*M23,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -3021,17 +3143,20 @@
         <v>0.40403</v>
       </c>
       <c r="M24">
-        <v>24.8</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="3"/>
-        <v>10</v>
+        <v>39.6</v>
       </c>
       <c r="O24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q24">
+        <f>ROUND(L24*M24,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -3060,17 +3185,20 @@
         <v>0.37841000000000002</v>
       </c>
       <c r="M25">
-        <v>42.3</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="3"/>
-        <v>16</v>
+        <v>44.9</v>
       </c>
       <c r="O25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25">
+        <f>ROUND(L25*M25,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -3101,15 +3229,18 @@
       <c r="M26">
         <v>2.7</v>
       </c>
-      <c r="N26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
       <c r="O26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q26">
+        <f>ROUND(L26*M26,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -3140,15 +3271,18 @@
       <c r="M27">
         <v>18.600000000000001</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
       <c r="O27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q27">
+        <f>ROUND(L27*M27,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3180,12 +3314,15 @@
         <f t="shared" si="2"/>
         <v>85.414100000000005</v>
       </c>
-      <c r="N28">
-        <f>SUM(N2:N27)</f>
-        <v>3008</v>
-      </c>
       <c r="O28" t="s">
         <v>26</v>
+      </c>
+      <c r="P28" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28">
+        <f>SUM(Q2:Q27)</f>
+        <v>3855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updatd JU, NW, NE, AG, VS, UR
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DBF428-B8F7-43AE-B525-7F03047C8D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D1B95A-FE83-4F59-A14D-B62FB73803A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="1515" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12690" yWindow="3180" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,6 +1633,9 @@
       <c r="A15" s="1">
         <v>43909</v>
       </c>
+      <c r="B15">
+        <v>118</v>
+      </c>
       <c r="C15">
         <v>3</v>
       </c>
@@ -1658,13 +1661,16 @@
         <v>123</v>
       </c>
       <c r="L15">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M15">
         <v>63</v>
       </c>
+      <c r="N15">
+        <v>132</v>
+      </c>
       <c r="O15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="P15">
         <v>17</v>
@@ -1687,11 +1693,14 @@
       <c r="V15">
         <v>638</v>
       </c>
+      <c r="W15">
+        <v>7</v>
+      </c>
       <c r="X15">
         <v>919</v>
       </c>
       <c r="Y15">
-        <v>176</v>
+        <v>232</v>
       </c>
       <c r="Z15">
         <v>23</v>
@@ -1747,7 +1756,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added data for 20. 3
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD89127F-8A22-49AF-976B-1105AD860562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266C91E7-C82B-469F-A511-5F61C12A2749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="2430" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5385" yWindow="2430" windowWidth="19080" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="62">
   <si>
     <t>ZH</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>@enno_hermann</t>
-  </si>
-  <si>
-    <t>https://www.coronavirus.bs.ch</t>
   </si>
   <si>
     <t>https://www.jura.ch/fr/Autorites/Coronavirus/Accueil/Coronavirus-Informations-officielles-a-la-population-jurassienne.html</t>
@@ -562,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1798,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>
@@ -1823,7 +1820,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>42</v>
@@ -1834,7 +1831,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1872,7 +1869,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>47</v>
@@ -1880,7 +1877,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>48</v>
@@ -1888,48 +1885,51 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>56</v>
@@ -1940,21 +1940,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1968,19 +1957,18 @@
     <hyperlink ref="B10" r:id="rId7" xr:uid="{A31E6CF7-91A7-4D97-B47D-3F52557EF47C}"/>
     <hyperlink ref="B9" r:id="rId8" xr:uid="{10400BC4-69C6-43F2-8E09-A52E1A451E9C}"/>
     <hyperlink ref="B11" r:id="rId9" xr:uid="{30961DFB-4E45-4611-A82F-A2689E420CC1}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{07F612FA-0C2F-4064-82BD-F93037B19CD8}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
-    <hyperlink ref="B8" r:id="rId19" xr:uid="{31E99BB6-82A4-4C45-B793-5F63A7878891}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
+    <hyperlink ref="B8" r:id="rId18" xr:uid="{31E99BB6-82A4-4C45-B793-5F63A7878891}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -2236,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q27" si="0">ROUND(L2*M2,0)</f>
@@ -2278,7 +2266,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
@@ -2320,7 +2308,7 @@
         <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
@@ -2362,7 +2350,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
@@ -2404,7 +2392,7 @@
         <v>16</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
@@ -2446,7 +2434,7 @@
         <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
@@ -2488,7 +2476,7 @@
         <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
@@ -2530,7 +2518,7 @@
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
@@ -2572,7 +2560,7 @@
         <v>22</v>
       </c>
       <c r="P10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
@@ -2614,7 +2602,7 @@
         <v>9</v>
       </c>
       <c r="P11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
@@ -2656,7 +2644,7 @@
         <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
@@ -2698,7 +2686,7 @@
         <v>19</v>
       </c>
       <c r="P13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
@@ -2740,7 +2728,7 @@
         <v>10</v>
       </c>
       <c r="P14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
@@ -2782,7 +2770,7 @@
         <v>17</v>
       </c>
       <c r="P15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
@@ -2824,7 +2812,7 @@
         <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
@@ -2866,7 +2854,7 @@
         <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
@@ -2908,7 +2896,7 @@
         <v>4</v>
       </c>
       <c r="P18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
@@ -2950,7 +2938,7 @@
         <v>8</v>
       </c>
       <c r="P19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
@@ -2992,7 +2980,7 @@
         <v>13</v>
       </c>
       <c r="P20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
@@ -3034,7 +3022,7 @@
         <v>25</v>
       </c>
       <c r="P21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
@@ -3076,7 +3064,7 @@
         <v>14</v>
       </c>
       <c r="P22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q22">
         <f t="shared" si="0"/>
@@ -3118,7 +3106,7 @@
         <v>6</v>
       </c>
       <c r="P23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
@@ -3160,7 +3148,7 @@
         <v>7</v>
       </c>
       <c r="P24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q24">
         <f t="shared" si="0"/>
@@ -3202,7 +3190,7 @@
         <v>5</v>
       </c>
       <c r="P25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q25">
         <f t="shared" si="0"/>
@@ -3244,7 +3232,7 @@
         <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
@@ -3286,7 +3274,7 @@
         <v>15</v>
       </c>
       <c r="P27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q27">
         <f t="shared" si="0"/>
@@ -3329,7 +3317,7 @@
         <v>26</v>
       </c>
       <c r="P28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q28">
         <f>SUM(Q2:Q27)</f>

</xml_diff>

<commit_message>
Updated TG, VD  and BS
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD3C0BA-D9A3-4860-8DEB-EF7CF94094A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C821F4-1B35-4C4F-B61E-36B4B2667EF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,9 +194,6 @@
     <t>* Official statement in video</t>
   </si>
   <si>
-    <t>https://www.24heures.ch/vaud-regions/Les-contaminations-sont-en-hausse-dans-le-canton-de-Vaud/story/23084946?cache=9efAwefu</t>
-  </si>
-  <si>
     <t>@f_giroud</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t xml:space="preserve">: </t>
+  </si>
+  <si>
+    <t>https://www.vd.ch/toutes-les-actualites/hotline-et-informations-sur-le-coronavirus/</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1611,7 @@
         <v>5</v>
       </c>
       <c r="X14">
-        <v>721</v>
+        <v>796</v>
       </c>
       <c r="Y14">
         <v>129</v>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="AB14" s="4">
         <f>SUM(B14:AA14)</f>
-        <v>3438</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>7</v>
       </c>
       <c r="X15">
-        <v>919</v>
+        <v>1001</v>
       </c>
       <c r="Y15">
         <v>232</v>
@@ -1708,17 +1708,25 @@
       </c>
       <c r="AB15">
         <f>SUM(B15:AA15)+I14</f>
-        <v>4281</v>
+        <v>4363</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
+      <c r="G16">
+        <v>272</v>
+      </c>
       <c r="Q16">
         <v>98</v>
       </c>
-      <c r="AB16" s="4"/>
+      <c r="U16">
+        <v>49</v>
+      </c>
+      <c r="AB16" s="4">
+        <v>4363</v>
+      </c>
     </row>
     <row r="17" spans="28:28" x14ac:dyDescent="0.25">
       <c r="AB17" s="4"/>
@@ -1761,7 +1769,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1812,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>
@@ -1826,7 +1834,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>42</v>
@@ -1837,7 +1845,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1908,10 +1916,10 @@
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,7 +1927,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,7 +1935,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
@@ -1938,7 +1946,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>42</v>
@@ -1949,7 +1957,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2230,7 +2238,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q27" si="0">ROUND(L2*M2,0)</f>
@@ -2272,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
@@ -2314,7 +2322,7 @@
         <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
@@ -2356,7 +2364,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
@@ -2398,7 +2406,7 @@
         <v>16</v>
       </c>
       <c r="P6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
@@ -2440,7 +2448,7 @@
         <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
@@ -2482,7 +2490,7 @@
         <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
@@ -2524,7 +2532,7 @@
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
@@ -2566,7 +2574,7 @@
         <v>22</v>
       </c>
       <c r="P10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
@@ -2608,7 +2616,7 @@
         <v>9</v>
       </c>
       <c r="P11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
@@ -2650,7 +2658,7 @@
         <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
@@ -2692,7 +2700,7 @@
         <v>19</v>
       </c>
       <c r="P13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
@@ -2734,7 +2742,7 @@
         <v>10</v>
       </c>
       <c r="P14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
@@ -2776,7 +2784,7 @@
         <v>17</v>
       </c>
       <c r="P15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
@@ -2818,7 +2826,7 @@
         <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
@@ -2860,7 +2868,7 @@
         <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
@@ -2902,7 +2910,7 @@
         <v>4</v>
       </c>
       <c r="P18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
@@ -2944,7 +2952,7 @@
         <v>8</v>
       </c>
       <c r="P19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
@@ -2986,7 +2994,7 @@
         <v>13</v>
       </c>
       <c r="P20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
@@ -3028,7 +3036,7 @@
         <v>25</v>
       </c>
       <c r="P21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
@@ -3070,7 +3078,7 @@
         <v>14</v>
       </c>
       <c r="P22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q22">
         <f t="shared" si="0"/>
@@ -3112,7 +3120,7 @@
         <v>6</v>
       </c>
       <c r="P23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
@@ -3154,7 +3162,7 @@
         <v>7</v>
       </c>
       <c r="P24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q24">
         <f t="shared" si="0"/>
@@ -3196,7 +3204,7 @@
         <v>5</v>
       </c>
       <c r="P25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q25">
         <f t="shared" si="0"/>
@@ -3238,7 +3246,7 @@
         <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
@@ -3280,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="P27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q27">
         <f t="shared" si="0"/>
@@ -3323,7 +3331,7 @@
         <v>26</v>
       </c>
       <c r="P28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q28">
         <f>SUM(Q2:Q27)</f>

</xml_diff>

<commit_message>
Updated UR and BL
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CB87E1-A5E1-4B25-9D65-62000C018EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA715651-74DA-4A52-8059-F6C854D2B003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3045" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+      <selection activeCell="I34" sqref="I34:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,7 +1725,7 @@
         <v>18</v>
       </c>
       <c r="F16">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="G16">
         <v>283</v>
@@ -1769,6 +1769,9 @@
       <c r="V16">
         <v>816</v>
       </c>
+      <c r="W16">
+        <v>7</v>
+      </c>
       <c r="X16">
         <v>1179</v>
       </c>
@@ -1780,7 +1783,7 @@
       </c>
       <c r="AB16" s="4">
         <f>SUM(B16:AA16)+Y15+W15+N15+I14+E15</f>
-        <v>4984</v>
+        <v>5008</v>
       </c>
     </row>
     <row r="17" spans="28:28" x14ac:dyDescent="0.25">
@@ -1823,7 +1826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated GE and AG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA715651-74DA-4A52-8059-F6C854D2B003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860B686D-7E86-423B-80E6-345B4F069309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3045" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6690" yWindow="3255" windowWidth="19080" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>https://www.jura.ch/fr/Autorites/Coronavirus/Accueil/Coronavirus-Informations-officielles-a-la-population-jurassienne.html</t>
   </si>
   <si>
-    <t>https://www.ge.ch/document/point-coronavirus-maladie-covid-19</t>
-  </si>
-  <si>
     <t>https://www.luzernerzeitung.ch/zentralschweiz/luzern/so-will-die-luzerner-regierung-die-massnahmen-des-bundes-umsetzen-lukb-stellt-50-millionen-franken-bereit-ld.1204954</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>https://www.baselland.ch/</t>
   </si>
   <si>
-    <t>https://www.ag.ch/de/themen_1/coronavirus_2/coronavirus.jsp</t>
-  </si>
-  <si>
     <t>https://www.coronavirus.bs.ch/</t>
   </si>
   <si>
@@ -222,6 +216,12 @@
   </si>
   <si>
     <t>https://www.vd.ch/toutes-les-actualites/hotline-et-informations-sur-le-coronavirus/</t>
+  </si>
+  <si>
+    <t>https://www.ag.ch/de/themen_1/coronavirus_2/alle_ereignisse/alle_ereignisse_1.jsp</t>
+  </si>
+  <si>
+    <t>https://www.ge.ch/document/point-coronavirus-maladie-covid-19, https://www.radiolac.ch/actualite/geneve-deux-nouveaux-deces-et-197-nouveaux-cas/</t>
   </si>
 </sst>
 </file>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34:J34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,6 +1652,9 @@
       <c r="H15">
         <v>82</v>
       </c>
+      <c r="I15">
+        <v>676</v>
+      </c>
       <c r="J15">
         <v>16</v>
       </c>
@@ -1708,7 +1711,7 @@
       </c>
       <c r="AB15">
         <f>SUM(B15:AA15)+I14</f>
-        <v>4363</v>
+        <v>5039</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -1716,7 +1719,7 @@
         <v>43910</v>
       </c>
       <c r="B16">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1733,6 +1736,9 @@
       <c r="H16">
         <v>109</v>
       </c>
+      <c r="I16">
+        <v>873</v>
+      </c>
       <c r="J16">
         <v>18</v>
       </c>
@@ -1782,8 +1788,8 @@
         <v>558</v>
       </c>
       <c r="AB16" s="4">
-        <f>SUM(B16:AA16)+Y15+W15+N15+I14+E15</f>
-        <v>5008</v>
+        <f>SUM(B16:AA16)+Y15+N15+E15</f>
+        <v>5439</v>
       </c>
     </row>
     <row r="17" spans="28:28" x14ac:dyDescent="0.25">
@@ -1826,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,7 +1876,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>
@@ -1892,7 +1898,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>42</v>
@@ -1903,7 +1909,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,7 +1958,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1960,13 +1966,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" t="s">
         <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1974,10 +1980,10 @@
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,7 +1991,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1993,7 +1999,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
@@ -2004,7 +2010,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>42</v>
@@ -2015,7 +2021,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2030,7 +2036,7 @@
     <hyperlink ref="B9" r:id="rId8" xr:uid="{10400BC4-69C6-43F2-8E09-A52E1A451E9C}"/>
     <hyperlink ref="B11" r:id="rId9" xr:uid="{30961DFB-4E45-4611-A82F-A2689E420CC1}"/>
     <hyperlink ref="B12" r:id="rId10" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.ge.ch/document/point-coronavirus-maladie-covid-19" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
     <hyperlink ref="B14" r:id="rId12" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
     <hyperlink ref="B15" r:id="rId13" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
@@ -2296,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q27" si="0">ROUND(L2*M2,0)</f>
@@ -2338,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
@@ -2380,7 +2386,7 @@
         <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
@@ -2422,7 +2428,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
@@ -2464,7 +2470,7 @@
         <v>16</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
@@ -2506,7 +2512,7 @@
         <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
@@ -2548,7 +2554,7 @@
         <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
@@ -2590,7 +2596,7 @@
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
@@ -2632,7 +2638,7 @@
         <v>22</v>
       </c>
       <c r="P10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
@@ -2674,7 +2680,7 @@
         <v>9</v>
       </c>
       <c r="P11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
@@ -2716,7 +2722,7 @@
         <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
@@ -2758,7 +2764,7 @@
         <v>19</v>
       </c>
       <c r="P13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
@@ -2800,7 +2806,7 @@
         <v>10</v>
       </c>
       <c r="P14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
@@ -2842,7 +2848,7 @@
         <v>17</v>
       </c>
       <c r="P15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
@@ -2884,7 +2890,7 @@
         <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
@@ -2926,7 +2932,7 @@
         <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
@@ -2968,7 +2974,7 @@
         <v>4</v>
       </c>
       <c r="P18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
@@ -3010,7 +3016,7 @@
         <v>8</v>
       </c>
       <c r="P19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
@@ -3052,7 +3058,7 @@
         <v>13</v>
       </c>
       <c r="P20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
@@ -3094,7 +3100,7 @@
         <v>25</v>
       </c>
       <c r="P21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
@@ -3136,7 +3142,7 @@
         <v>14</v>
       </c>
       <c r="P22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q22">
         <f t="shared" si="0"/>
@@ -3178,7 +3184,7 @@
         <v>6</v>
       </c>
       <c r="P23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
@@ -3220,7 +3226,7 @@
         <v>7</v>
       </c>
       <c r="P24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q24">
         <f t="shared" si="0"/>
@@ -3262,7 +3268,7 @@
         <v>5</v>
       </c>
       <c r="P25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q25">
         <f t="shared" si="0"/>
@@ -3304,7 +3310,7 @@
         <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
@@ -3346,7 +3352,7 @@
         <v>15</v>
       </c>
       <c r="P27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q27">
         <f t="shared" si="0"/>
@@ -3389,7 +3395,7 @@
         <v>26</v>
       </c>
       <c r="P28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q28">
         <f>SUM(Q2:Q27)</f>

</xml_diff>

<commit_message>
Update GE, VD, TI, ZG, VS
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4683399E-A87C-490B-8D9A-4F9666C2F771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E659F16-8AC7-49E1-B60B-442D3F2FE7BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="3225" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6075" yWindow="1920" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="63">
   <si>
     <t>ZH</t>
   </si>
@@ -182,9 +182,6 @@
     <t>https://www.jura.ch/fr/Autorites/Coronavirus/Accueil/Coronavirus-Informations-officielles-a-la-population-jurassienne.html</t>
   </si>
   <si>
-    <t>https://www.luzernerzeitung.ch/zentralschweiz/luzern/so-will-die-luzerner-regierung-die-massnahmen-des-bundes-umsetzen-lukb-stellt-50-millionen-franken-bereit-ld.1204954</t>
-  </si>
-  <si>
     <t>@neph_b</t>
   </si>
   <si>
@@ -222,6 +219,12 @@
   </si>
   <si>
     <t>https://www.ge.ch/document/point-coronavirus-maladie-covid-19, https://www.radiolac.ch/actualite/geneve-deux-nouveaux-deces-et-197-nouveaux-cas/</t>
+  </si>
+  <si>
+    <t>https://gesundheit.lu.ch/themen/Humanmedizin/Infektionskrankheiten/Coronavirus</t>
+  </si>
+  <si>
+    <t>https://www.zg.ch/behoerden/gesundheitsdirektion/direktionssekretariat/aktuell/coronavirus-ausreichende-testkapazitaeten-im-kanton-zug-vorhanden</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="X11">
-        <v>331</v>
+        <v>406</v>
       </c>
       <c r="AB11" s="4">
         <v>2155</v>
@@ -1487,7 +1490,7 @@
         <v>330</v>
       </c>
       <c r="X12">
-        <v>461</v>
+        <v>508</v>
       </c>
       <c r="AA12">
         <v>270</v>
@@ -1528,7 +1531,7 @@
         <v>422</v>
       </c>
       <c r="X13">
-        <v>695</v>
+        <v>608</v>
       </c>
       <c r="Y13">
         <v>95</v>
@@ -1659,7 +1662,7 @@
         <v>16</v>
       </c>
       <c r="K15">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="L15">
         <v>27</v>
@@ -1698,7 +1701,7 @@
         <v>7</v>
       </c>
       <c r="X15">
-        <v>1001</v>
+        <v>1212</v>
       </c>
       <c r="Y15">
         <v>232</v>
@@ -1710,8 +1713,8 @@
         <v>526</v>
       </c>
       <c r="AB15">
-        <f>SUM(B15:AA15)+I14</f>
-        <v>5039</v>
+        <f>SUM(B15:AA15)</f>
+        <v>4804</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -1728,13 +1731,13 @@
         <v>18</v>
       </c>
       <c r="E16">
-        <v>238</v>
+        <v>377</v>
       </c>
       <c r="F16">
         <v>184</v>
       </c>
       <c r="G16">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="H16">
         <v>109</v>
@@ -1752,13 +1755,13 @@
         <v>29</v>
       </c>
       <c r="M16">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="N16">
         <v>159</v>
       </c>
       <c r="O16">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P16">
         <v>17</v>
@@ -1767,7 +1770,7 @@
         <v>98</v>
       </c>
       <c r="R16">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="S16">
         <v>46</v>
@@ -1785,17 +1788,20 @@
         <v>7</v>
       </c>
       <c r="X16">
-        <v>1179</v>
+        <v>1212</v>
+      </c>
+      <c r="Y16">
+        <v>282</v>
       </c>
       <c r="Z16">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="AA16">
         <v>558</v>
       </c>
       <c r="AB16" s="4">
-        <f>SUM(B16:AA16)+Y15+N15+E15</f>
-        <v>5836</v>
+        <f>SUM(B16:AA16)</f>
+        <v>5675</v>
       </c>
     </row>
     <row r="17" spans="28:28" x14ac:dyDescent="0.25">
@@ -1836,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +1888,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>
@@ -1904,7 +1910,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>42</v>
@@ -1915,7 +1921,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1964,7 +1970,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,13 +1978,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,10 +1992,10 @@
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1997,7 +2003,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2005,7 +2011,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
@@ -2016,7 +2022,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>42</v>
@@ -2027,7 +2033,15 @@
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2050,9 +2064,10 @@
     <hyperlink ref="B18" r:id="rId16" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
     <hyperlink ref="B19" r:id="rId17" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
     <hyperlink ref="B8" r:id="rId18" xr:uid="{31E99BB6-82A4-4C45-B793-5F63A7878891}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{1EAFE4A5-0491-4F61-9BF3-31053EEEC247}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -2308,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q27" si="0">ROUND(L2*M2,0)</f>
@@ -2350,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
@@ -2392,7 +2407,7 @@
         <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
@@ -2434,7 +2449,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
@@ -2476,7 +2491,7 @@
         <v>16</v>
       </c>
       <c r="P6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
@@ -2518,7 +2533,7 @@
         <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
@@ -2560,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
@@ -2602,7 +2617,7 @@
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
@@ -2644,7 +2659,7 @@
         <v>22</v>
       </c>
       <c r="P10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
@@ -2686,7 +2701,7 @@
         <v>9</v>
       </c>
       <c r="P11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
@@ -2728,7 +2743,7 @@
         <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
@@ -2770,7 +2785,7 @@
         <v>19</v>
       </c>
       <c r="P13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
@@ -2812,7 +2827,7 @@
         <v>10</v>
       </c>
       <c r="P14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
@@ -2854,7 +2869,7 @@
         <v>17</v>
       </c>
       <c r="P15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
@@ -2896,7 +2911,7 @@
         <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
@@ -2938,7 +2953,7 @@
         <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
@@ -2980,7 +2995,7 @@
         <v>4</v>
       </c>
       <c r="P18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
@@ -3022,7 +3037,7 @@
         <v>8</v>
       </c>
       <c r="P19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
@@ -3064,7 +3079,7 @@
         <v>13</v>
       </c>
       <c r="P20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
@@ -3106,7 +3121,7 @@
         <v>25</v>
       </c>
       <c r="P21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
@@ -3148,7 +3163,7 @@
         <v>14</v>
       </c>
       <c r="P22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q22">
         <f t="shared" si="0"/>
@@ -3190,7 +3205,7 @@
         <v>6</v>
       </c>
       <c r="P23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
@@ -3232,7 +3247,7 @@
         <v>7</v>
       </c>
       <c r="P24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q24">
         <f t="shared" si="0"/>
@@ -3274,7 +3289,7 @@
         <v>5</v>
       </c>
       <c r="P25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q25">
         <f t="shared" si="0"/>
@@ -3316,7 +3331,7 @@
         <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
@@ -3358,7 +3373,7 @@
         <v>15</v>
       </c>
       <c r="P27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q27">
         <f t="shared" si="0"/>
@@ -3401,7 +3416,7 @@
         <v>26</v>
       </c>
       <c r="P28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q28">
         <f>SUM(Q2:Q27)</f>

</xml_diff>

<commit_message>
Updated BS and TI
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91036E82-B79E-467B-89CC-985DCD3FB203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A3476A-80D7-43F4-90AE-71735B01A1E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="1920" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="1200" windowWidth="19080" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,7 +1824,7 @@
         <v>184</v>
       </c>
       <c r="G17">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="H17">
         <v>109</v>
@@ -1869,7 +1869,7 @@
         <v>49</v>
       </c>
       <c r="V17">
-        <v>834</v>
+        <v>918</v>
       </c>
       <c r="W17">
         <v>7</v>
@@ -1928,7 +1928,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated VD for 20.03.
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8515A8E5-1E47-455A-8830-F2CDCB957ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0B2D16-1D10-4F2C-B0B3-42A56343DE30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="1200" windowWidth="24255" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
-    <sheet name="Quellen" sheetId="4" r:id="rId2"/>
-    <sheet name="Tests" sheetId="5" r:id="rId3"/>
-    <sheet name="demographics" sheetId="3" r:id="rId4"/>
+    <sheet name="covid19_fatalities_switzerland" sheetId="6" r:id="rId2"/>
+    <sheet name="Quellen" sheetId="4" r:id="rId3"/>
+    <sheet name="Tests" sheetId="5" r:id="rId4"/>
+    <sheet name="demographics" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="63">
   <si>
     <t>ZH</t>
   </si>
@@ -563,7 +564,7 @@
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,7 +1789,7 @@
         <v>7</v>
       </c>
       <c r="X16">
-        <v>1212</v>
+        <v>1432</v>
       </c>
       <c r="Y16">
         <v>282</v>
@@ -1801,7 +1802,7 @@
       </c>
       <c r="AB16" s="4">
         <f>SUM(B16:AA16)</f>
-        <v>5908</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -1816,7 +1817,7 @@
       </c>
       <c r="AB17" s="4">
         <f>SUM(W16:AA16)+SUM(H16:U16)+SUM(B16:F16)+V17+G17</f>
-        <v>6019</v>
+        <v>6239</v>
       </c>
     </row>
   </sheetData>
@@ -1829,6 +1830,244 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
+  <dimension ref="A1:AB17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y21" sqref="Y21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43896</v>
+      </c>
+      <c r="AB2" s="4"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43897</v>
+      </c>
+      <c r="AB3" s="4"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43898</v>
+      </c>
+      <c r="AB4" s="4"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43899</v>
+      </c>
+      <c r="AB5" s="4"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43900</v>
+      </c>
+      <c r="AB6" s="4"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43901</v>
+      </c>
+      <c r="AB7" s="4"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43902</v>
+      </c>
+      <c r="AB8" s="4"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43903</v>
+      </c>
+      <c r="AB9" s="4"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43904</v>
+      </c>
+      <c r="AB10" s="4"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43905</v>
+      </c>
+      <c r="AB11" s="4"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43906</v>
+      </c>
+      <c r="AB12" s="5"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43907</v>
+      </c>
+      <c r="AB13" s="4"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43908</v>
+      </c>
+      <c r="AB14" s="4"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43910</v>
+      </c>
+      <c r="AB16" s="4"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43911</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>28</v>
+      </c>
+      <c r="X17">
+        <v>12</v>
+      </c>
+      <c r="AB17" s="4">
+        <f>SUM(B17:AA17)</f>
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -2059,7 +2298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB15D9C-377E-4F66-998B-5427F83AE200}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
@@ -2239,7 +2478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31030D7-6127-45B4-88E3-D01E088D3FDA}">
   <dimension ref="A1:Q28"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated BE and GR
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1ACA22-6557-4734-8C8D-9CC7DC585392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F65A98D-20A4-4F88-89D8-4B544F29E082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1890" windowWidth="24255" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="2895" windowWidth="24255" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1842,7 @@
         <v>22</v>
       </c>
       <c r="E17">
-        <v>377</v>
+        <v>418</v>
       </c>
       <c r="F17">
         <v>282</v>
@@ -1860,13 +1860,13 @@
         <v>21</v>
       </c>
       <c r="K17">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="L17">
         <v>49</v>
       </c>
       <c r="M17">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="N17">
         <v>177</v>
@@ -1906,7 +1906,16 @@
       </c>
       <c r="AB17" s="4">
         <f>SUM(B17:AA17)+AA16+Z16</f>
-        <v>6828</v>
+        <v>6912</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43912</v>
+      </c>
+      <c r="AB18" s="4">
+        <f>AB17</f>
+        <v>6912</v>
       </c>
     </row>
   </sheetData>
@@ -1922,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2323,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated BS and TG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F122BE70-79D6-4B58-92BB-6676834861FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B198ECB-EC21-4A49-B88D-2E343DE09428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="2895" windowWidth="24255" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="2895" windowWidth="24255" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,9 +1913,15 @@
       <c r="A18" s="1">
         <v>43912</v>
       </c>
+      <c r="G18">
+        <v>358</v>
+      </c>
+      <c r="U18">
+        <v>75</v>
+      </c>
       <c r="AB18" s="4">
-        <f>AB17</f>
-        <v>6912</v>
+        <f>AB17+G18-G17+U18-U17</f>
+        <v>6990</v>
       </c>
     </row>
   </sheetData>
@@ -1931,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:L25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated BL and LU
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9612293A-7174-482E-BA55-2C2CEE0FE851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE99B4BB-C8CD-4A50-BE81-47D28D97EC3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="2385" windowWidth="20235" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,6 +1922,9 @@
       <c r="D18">
         <v>26</v>
       </c>
+      <c r="F18">
+        <v>289</v>
+      </c>
       <c r="G18">
         <v>358</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>24</v>
       </c>
       <c r="M18">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="P18">
         <v>20</v>
@@ -1962,8 +1965,8 @@
         <v>891</v>
       </c>
       <c r="AB18" s="4">
-        <f>SUM(B18:AA18)+Z16+X17+W17+O17+N17+L17+K17+I17+F17+E17</f>
-        <v>7534</v>
+        <f>SUM(B18:AA18)+Z16+X17+W17+O17+N17+L17+K17+I17+E17</f>
+        <v>7549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated NW, VS, and JU
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42867089-3A76-4E08-9109-511216E33FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFB4812-96DE-408B-A0A3-61ABDDE0B984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="1860" windowWidth="20235" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="2070" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,12 +1940,18 @@
       <c r="K18">
         <v>257</v>
       </c>
+      <c r="L18">
+        <v>51</v>
+      </c>
       <c r="M18">
         <v>131</v>
       </c>
       <c r="N18">
         <v>188</v>
       </c>
+      <c r="O18">
+        <v>36</v>
+      </c>
       <c r="P18">
         <v>20</v>
       </c>
@@ -1968,14 +1974,14 @@
         <v>939</v>
       </c>
       <c r="Y18">
-        <v>385</v>
+        <v>432</v>
       </c>
       <c r="AA18">
         <v>891</v>
       </c>
       <c r="AB18" s="4">
-        <f>SUM(B18:AA18)+Z16+X17+W17+O17+L17+E17</f>
-        <v>7674</v>
+        <f>SUM(B18:AA18)+Z16+X17+W17+E17</f>
+        <v>7726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BE, and SG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F338B0-C7D0-41F6-A053-1CC11167D69D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C935CF5E-EB0F-4D61-BA19-FA7C485BF058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="2235" windowWidth="22290" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="2235" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,6 +1984,24 @@
         <v>7726</v>
       </c>
     </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43913</v>
+      </c>
+      <c r="E19">
+        <v>470</v>
+      </c>
+      <c r="K19">
+        <v>266</v>
+      </c>
+      <c r="Q19">
+        <v>185</v>
+      </c>
+      <c r="AB19" s="4">
+        <f>AB18+Q19-Q18+K19-K18+E19-E17</f>
+        <v>7809</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U5:U17">
     <sortCondition ref="U5"/>
@@ -1995,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2502,6 +2520,54 @@
         <v>99</v>
       </c>
     </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>13</v>
+      </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <v>37</v>
+      </c>
+      <c r="X19">
+        <v>15</v>
+      </c>
+      <c r="Y19">
+        <v>10</v>
+      </c>
+      <c r="AA19">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="4">
+        <f>SUM(B19:AA19)</f>
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2512,7 +2578,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated TG and LU
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93C6CBE-D5F7-45A6-983A-73DB93EE66A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A5AC33-CB65-4DA9-9409-64627FF82C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="2235" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15825" yWindow="2295" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,9 +1994,15 @@
       <c r="K19">
         <v>266</v>
       </c>
+      <c r="M19">
+        <v>156</v>
+      </c>
       <c r="Q19">
         <v>185</v>
       </c>
+      <c r="U19">
+        <v>81</v>
+      </c>
       <c r="V19">
         <v>1165</v>
       </c>
@@ -2004,8 +2010,8 @@
         <v>1068</v>
       </c>
       <c r="AB19" s="4">
-        <f>AB18+Q19-Q18+K19-K18+E19-E17+V19-V18+AA19-AA18</f>
-        <v>8227</v>
+        <f>AB18+Q19-Q18+K19-K18+E19-E17+V19-V18+AA19-AA18+U19-U18+M19-M18</f>
+        <v>8258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated SH and UR
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A5AC33-CB65-4DA9-9409-64627FF82C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F831DEF-F2CD-48D0-8047-855F90CE128F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15825" yWindow="2295" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="2985" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -228,10 +228,10 @@
     <t>https://www.ur.ch/themen/2920</t>
   </si>
   <si>
-    <t>https://www.ge.ch/covid-19-coronavirus-geneve/situation-epidemiologique-geneve</t>
-  </si>
-  <si>
     <t>@ThomasGriessen</t>
+  </si>
+  <si>
+    <t>https://www.ge.ch/covid-19-professionnels-sante-reseau-soins</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="M24" sqref="M23:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,6 +1973,9 @@
       <c r="V18">
         <v>939</v>
       </c>
+      <c r="W18">
+        <v>12</v>
+      </c>
       <c r="Y18">
         <v>432</v>
       </c>
@@ -1981,7 +1984,7 @@
       </c>
       <c r="AB18" s="4">
         <f>SUM(B18:AA18)+Z16+X17+W17+E17</f>
-        <v>7741</v>
+        <v>7753</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -2000,18 +2003,24 @@
       <c r="Q19">
         <v>185</v>
       </c>
+      <c r="R19">
+        <v>30</v>
+      </c>
       <c r="U19">
         <v>81</v>
       </c>
       <c r="V19">
         <v>1165</v>
       </c>
+      <c r="W19">
+        <v>12</v>
+      </c>
       <c r="AA19">
         <v>1068</v>
       </c>
       <c r="AB19" s="4">
-        <f>AB18+Q19-Q18+K19-K18+E19-E17+V19-V18+AA19-AA18+U19-U18+M19-M18</f>
-        <v>8258</v>
+        <f>AB18+Q19-Q18+K19-K18+E19-E17+V19-V18+AA19-AA18+U19-U18+M19-M18+R19-R18</f>
+        <v>8272</v>
       </c>
     </row>
   </sheetData>
@@ -2589,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7CD16-821B-4F71-9E45-F399140EBC9C}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2716,10 +2725,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2814,15 +2823,15 @@
     <hyperlink ref="B11" r:id="rId9" xr:uid="{30961DFB-4E45-4611-A82F-A2689E420CC1}"/>
     <hyperlink ref="B12" r:id="rId10" xr:uid="{7691208C-FFDC-4FF8-92C7-35AF3F7D70C3}"/>
     <hyperlink ref="B13" r:id="rId11" xr:uid="{E1CE2206-BBEB-46B5-9776-F8AFE6FF73B7}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
-    <hyperlink ref="B8" r:id="rId18" xr:uid="{31E99BB6-82A4-4C45-B793-5F63A7878891}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{1EAFE4A5-0491-4F61-9BF3-31053EEEC247}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{D97958E5-3E9B-4AE6-83ED-1BD900EA7199}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{BB97D922-F236-484B-9A6A-5EC1C87ED5F6}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{5E4E04C7-A68C-4DC8-9547-5DA33AB3469E}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{6D3273C1-5FFA-4B84-8BD6-E04F2ABC952F}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{BD05A047-E32B-4A12-BE51-6351F4C7C42F}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{38512648-04E5-4491-96AA-EF48D53636AB}"/>
+    <hyperlink ref="B8" r:id="rId17" xr:uid="{31E99BB6-82A4-4C45-B793-5F63A7878891}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{1EAFE4A5-0491-4F61-9BF3-31053EEEC247}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{D97958E5-3E9B-4AE6-83ED-1BD900EA7199}"/>
+    <hyperlink ref="B14" r:id="rId20" xr:uid="{EDD4802E-432B-4800-A01A-91A6027A11EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>

</xml_diff>

<commit_message>
Updated from BAG incidences
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5F27F8-6C58-4CED-B7A0-44D4CABA018C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADD9E31-9B1E-4413-87F9-B65D444708CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="2985" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="3195" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,21 +1991,51 @@
       <c r="A19" s="1">
         <v>43913</v>
       </c>
+      <c r="B19">
+        <v>234</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>27</v>
+      </c>
       <c r="E19">
         <v>470</v>
       </c>
+      <c r="F19">
+        <v>292</v>
+      </c>
+      <c r="G19">
+        <v>376</v>
+      </c>
+      <c r="H19">
+        <v>189</v>
+      </c>
+      <c r="J19">
+        <v>29</v>
+      </c>
       <c r="K19">
         <v>266</v>
       </c>
       <c r="M19">
         <v>156</v>
       </c>
+      <c r="P19">
+        <v>21</v>
+      </c>
       <c r="Q19">
         <v>185</v>
       </c>
       <c r="R19">
         <v>30</v>
       </c>
+      <c r="S19">
+        <v>83</v>
+      </c>
+      <c r="T19">
+        <v>73</v>
+      </c>
       <c r="U19">
         <v>81</v>
       </c>
@@ -2015,12 +2045,18 @@
       <c r="W19">
         <v>12</v>
       </c>
+      <c r="X19">
+        <v>1880</v>
+      </c>
+      <c r="Y19">
+        <v>441</v>
+      </c>
       <c r="AA19">
         <v>1068</v>
       </c>
       <c r="AB19" s="4">
-        <f>AB18+Q19-Q18+K19-K18+E19-E17+V19-V18+AA19-AA18+U19-U18+M19-M18+R19-R18</f>
-        <v>8260</v>
+        <f>SUM(B19:AA19)+Z16+O18+N18+L18+I18</f>
+        <v>8549</v>
       </c>
     </row>
   </sheetData>
@@ -2599,7 +2635,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3084,7 +3120,7 @@
         <v>15.209680000000001</v>
       </c>
       <c r="M2">
-        <v>58.6</v>
+        <v>62.8</v>
       </c>
       <c r="O2" t="s">
         <v>0</v>
@@ -3094,7 +3130,7 @@
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q27" si="0">ROUND(L2*M2,0)</f>
-        <v>891</v>
+        <v>955</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -3126,7 +3162,7 @@
         <v>10.349769999999999</v>
       </c>
       <c r="M3">
-        <v>39.5</v>
+        <v>43</v>
       </c>
       <c r="O3" t="s">
         <v>1</v>
@@ -3136,7 +3172,7 @@
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>409</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -3168,7 +3204,7 @@
         <v>7.9914500000000004</v>
       </c>
       <c r="M4">
-        <v>205.8</v>
+        <v>235.3</v>
       </c>
       <c r="O4" t="s">
         <v>21</v>
@@ -3178,7 +3214,7 @@
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>1645</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3210,7 +3246,7 @@
         <v>6.78207</v>
       </c>
       <c r="M5">
-        <v>32</v>
+        <v>34.5</v>
       </c>
       <c r="O5" t="s">
         <v>18</v>
@@ -3220,7 +3256,7 @@
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>217</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -3252,7 +3288,7 @@
         <v>5.0769700000000002</v>
       </c>
       <c r="M6">
-        <v>32.1</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="O6" t="s">
         <v>16</v>
@@ -3262,7 +3298,7 @@
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>163</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -3294,7 +3330,7 @@
         <v>4.9524900000000001</v>
       </c>
       <c r="M7">
-        <v>96.9</v>
+        <v>136.30000000000001</v>
       </c>
       <c r="O7" t="s">
         <v>24</v>
@@ -3304,7 +3340,7 @@
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>675</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -3336,7 +3372,7 @@
         <v>4.0955700000000004</v>
       </c>
       <c r="M8">
-        <v>30</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="O8" t="s">
         <v>2</v>
@@ -3346,7 +3382,7 @@
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -3378,7 +3414,7 @@
         <v>3.5334300000000001</v>
       </c>
       <c r="M9">
-        <v>263.5</v>
+        <v>326.89999999999998</v>
       </c>
       <c r="O9" t="s">
         <v>20</v>
@@ -3388,7 +3424,7 @@
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>931</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3420,7 +3456,7 @@
         <v>3.4395500000000001</v>
       </c>
       <c r="M10">
-        <v>111.9</v>
+        <v>128.19999999999999</v>
       </c>
       <c r="O10" t="s">
         <v>22</v>
@@ -3430,7 +3466,7 @@
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
-        <v>385</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -3462,7 +3498,7 @@
         <v>3.1871399999999999</v>
       </c>
       <c r="M11">
-        <v>50.8</v>
+        <v>59.3</v>
       </c>
       <c r="O11" t="s">
         <v>9</v>
@@ -3472,7 +3508,7 @@
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
-        <v>162</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -3504,7 +3540,7 @@
         <v>2.8813200000000001</v>
       </c>
       <c r="M12">
-        <v>97.2</v>
+        <v>101.3</v>
       </c>
       <c r="O12" t="s">
         <v>12</v>
@@ -3514,7 +3550,7 @@
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -3546,7 +3582,7 @@
         <v>2.7647200000000001</v>
       </c>
       <c r="M13">
-        <v>19.899999999999999</v>
+        <v>23.9</v>
       </c>
       <c r="O13" t="s">
         <v>19</v>
@@ -3556,7 +3592,7 @@
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -3588,7 +3624,7 @@
         <v>2.7319399999999998</v>
       </c>
       <c r="M14">
-        <v>24.9</v>
+        <v>30.4</v>
       </c>
       <c r="O14" t="s">
         <v>10</v>
@@ -3598,7 +3634,7 @@
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -3630,7 +3666,7 @@
         <v>1.9837899999999999</v>
       </c>
       <c r="M15">
-        <v>118.5</v>
+        <v>133.6</v>
       </c>
       <c r="O15" t="s">
         <v>17</v>
@@ -3640,7 +3676,7 @@
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -3672,7 +3708,7 @@
         <v>1.9476599999999999</v>
       </c>
       <c r="M16">
-        <v>203.8</v>
+        <v>222.8</v>
       </c>
       <c r="O16" t="s">
         <v>11</v>
@@ -3682,7 +3718,7 @@
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
-        <v>397</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -3714,7 +3750,7 @@
         <v>1.7796400000000001</v>
       </c>
       <c r="M17">
-        <v>82</v>
+        <v>84.3</v>
       </c>
       <c r="O17" t="s">
         <v>23</v>
@@ -3724,7 +3760,7 @@
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -3756,7 +3792,7 @@
         <v>1.59165</v>
       </c>
       <c r="M18">
-        <v>44</v>
+        <v>45.9</v>
       </c>
       <c r="O18" t="s">
         <v>4</v>
@@ -3766,7 +3802,7 @@
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -3798,7 +3834,7 @@
         <v>1.26837</v>
       </c>
       <c r="M19">
-        <v>30.7</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="O19" t="s">
         <v>8</v>
@@ -3808,7 +3844,7 @@
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -3840,7 +3876,7 @@
         <v>0.81991000000000003</v>
       </c>
       <c r="M20">
-        <v>34.200000000000003</v>
+        <v>36.6</v>
       </c>
       <c r="O20" t="s">
         <v>13</v>
@@ -3850,7 +3886,7 @@
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -3882,7 +3918,7 @@
         <v>0.73419000000000001</v>
       </c>
       <c r="M21">
-        <v>65.400000000000006</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="O21" t="s">
         <v>25</v>
@@ -3892,7 +3928,7 @@
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -3924,7 +3960,7 @@
         <v>0.55234000000000005</v>
       </c>
       <c r="M22">
-        <v>47.1</v>
+        <v>48.9</v>
       </c>
       <c r="O22" t="s">
         <v>14</v>
@@ -3934,7 +3970,7 @@
       </c>
       <c r="Q22">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -3966,7 +4002,7 @@
         <v>0.43223</v>
       </c>
       <c r="M23">
-        <v>74</v>
+        <v>78.7</v>
       </c>
       <c r="O23" t="s">
         <v>6</v>
@@ -3976,7 +4012,7 @@
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -4008,7 +4044,7 @@
         <v>0.40403</v>
       </c>
       <c r="M24">
-        <v>59.4</v>
+        <v>71.8</v>
       </c>
       <c r="O24" t="s">
         <v>7</v>
@@ -4018,7 +4054,7 @@
       </c>
       <c r="Q24">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -4050,7 +4086,7 @@
         <v>0.37841000000000002</v>
       </c>
       <c r="M25">
-        <v>52.9</v>
+        <v>55.5</v>
       </c>
       <c r="O25" t="s">
         <v>5</v>
@@ -4060,7 +4096,7 @@
       </c>
       <c r="Q25">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -4092,7 +4128,7 @@
         <v>0.36432999999999999</v>
       </c>
       <c r="M26">
-        <v>24.7</v>
+        <v>49.4</v>
       </c>
       <c r="O26" t="s">
         <v>3</v>
@@ -4102,7 +4138,7 @@
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -4134,7 +4170,7 @@
         <v>0.16145000000000001</v>
       </c>
       <c r="M27">
-        <v>18.600000000000001</v>
+        <v>24.8</v>
       </c>
       <c r="O27" t="s">
         <v>15</v>
@@ -4144,7 +4180,7 @@
       </c>
       <c r="Q27">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -4187,7 +4223,7 @@
       </c>
       <c r="Q28">
         <f>SUM(Q2:Q27)</f>
-        <v>6886</v>
+        <v>7920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GR and ZG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65236226-16A8-4639-A3E6-EB13621F04A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBCBB77-A800-4828-9196-B25CF02BD2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12615" yWindow="2460" windowWidth="22290" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8370" yWindow="2550" windowWidth="22290" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2040,7 @@
         <v>25</v>
       </c>
       <c r="Q19">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="R19">
         <v>30</v>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="AB19" s="4">
         <f>SUM(B19:AA19)</f>
-        <v>8781</v>
+        <v>8796</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -2082,11 +2082,14 @@
         <v>43914</v>
       </c>
       <c r="K20">
-        <v>296</v>
+        <v>276</v>
+      </c>
+      <c r="Z20">
+        <v>72</v>
       </c>
       <c r="AB20" s="4">
-        <f>AB19+K20-K19</f>
-        <v>8811</v>
+        <f>AB19+K20-K19+Z20-Z19</f>
+        <v>8816</v>
       </c>
     </row>
   </sheetData>
@@ -2102,7 +2105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated VS, JU, TG, BL
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075B2945-EE0C-41A7-B6D0-49DE9BFD8F0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777A74E7-8CB7-4ADE-B293-956A390FE322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1035" windowWidth="18900" windowHeight="19665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="1035" windowWidth="18900" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,6 +2109,9 @@
       <c r="K20">
         <v>276</v>
       </c>
+      <c r="L20">
+        <v>66</v>
+      </c>
       <c r="M20">
         <v>205</v>
       </c>
@@ -2118,6 +2121,9 @@
       <c r="O20">
         <v>42</v>
       </c>
+      <c r="P20">
+        <v>25</v>
+      </c>
       <c r="Q20">
         <v>203</v>
       </c>
@@ -2143,8 +2149,8 @@
         <v>1211</v>
       </c>
       <c r="AB20" s="4">
-        <f>SUM(B20:AA20)+X19+W19+S19+P19+L19</f>
-        <v>9875</v>
+        <f>SUM(B20:AA20)+X19+W19+S19</f>
+        <v>9884</v>
       </c>
     </row>
   </sheetData>
@@ -2160,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2733,7 +2739,7 @@
         <v>6</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G20">
         <v>5</v>
@@ -2756,6 +2762,9 @@
       <c r="S20">
         <v>1</v>
       </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
       <c r="V20">
         <v>53</v>
       </c>
@@ -2770,7 +2779,7 @@
       </c>
       <c r="AB20" s="4">
         <f>SUM(B20:AA20)</f>
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last update of today
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777A74E7-8CB7-4ADE-B293-956A390FE322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F75BD2F-4C3E-4D90-B30D-1FDBDC41B712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1035" windowWidth="18900" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="1035" windowWidth="18900" windowHeight="19665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,7 +2017,7 @@
         <v>1509</v>
       </c>
       <c r="J19">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K19">
         <v>266</v>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="AB19" s="4">
         <f>SUM(B19:AA19)</f>
-        <v>9356</v>
+        <v>9358</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -2083,10 +2083,10 @@
         <v>266</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E20">
         <v>532</v>
@@ -2104,7 +2104,7 @@
         <v>1510</v>
       </c>
       <c r="J20">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K20">
         <v>276</v>
@@ -2139,6 +2139,9 @@
       <c r="V20">
         <v>1211</v>
       </c>
+      <c r="W20">
+        <v>25</v>
+      </c>
       <c r="Y20">
         <v>544</v>
       </c>
@@ -2149,8 +2152,8 @@
         <v>1211</v>
       </c>
       <c r="AB20" s="4">
-        <f>SUM(B20:AA20)+X19+W19+S19</f>
-        <v>9884</v>
+        <f>SUM(B20:AA20)+X19+S19</f>
+        <v>9896</v>
       </c>
     </row>
   </sheetData>
@@ -2166,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W29" sqref="W29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,7 +2772,7 @@
         <v>53</v>
       </c>
       <c r="X20">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Y20">
         <v>13</v>
@@ -2779,7 +2782,7 @@
       </c>
       <c r="AB20" s="4">
         <f>SUM(B20:AA20)</f>
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BE and ZG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F75BD2F-4C3E-4D90-B30D-1FDBDC41B712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BBE66F-DCF7-42A3-9584-6093AC3E7274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1035" windowWidth="18900" windowHeight="19665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17085" yWindow="810" windowWidth="18900" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,6 +2130,9 @@
       <c r="R20">
         <v>32</v>
       </c>
+      <c r="S20">
+        <v>129</v>
+      </c>
       <c r="T20">
         <v>80</v>
       </c>
@@ -2152,8 +2155,23 @@
         <v>1211</v>
       </c>
       <c r="AB20" s="4">
-        <f>SUM(B20:AA20)+X19+S19</f>
-        <v>9896</v>
+        <f>SUM(B20:AA20)+X19</f>
+        <v>9921</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43915</v>
+      </c>
+      <c r="E21">
+        <v>624</v>
+      </c>
+      <c r="Z21">
+        <v>80</v>
+      </c>
+      <c r="AB21" s="4">
+        <f>AB20+E21-E20+Z21-Z20</f>
+        <v>10021</v>
       </c>
     </row>
   </sheetData>
@@ -2167,10 +2185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2782,6 +2800,63 @@
       </c>
       <c r="AB20" s="4">
         <f>SUM(B20:AA20)</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>53</v>
+      </c>
+      <c r="X21">
+        <v>17</v>
+      </c>
+      <c r="Y21">
+        <v>13</v>
+      </c>
+      <c r="AA21">
+        <v>5</v>
+      </c>
+      <c r="AB21" s="4">
+        <f>SUM(B21:AA21)</f>
         <v>131</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated VS, JU, SZ
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B0E2E4-02FE-4D5F-BFF3-A67B041E045E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0F03FD-AD98-4A81-B65F-9159475B72F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17235" yWindow="1335" windowWidth="19470" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17235" yWindow="1335" windowWidth="19470" windowHeight="19665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,6 +2190,9 @@
       <c r="K21">
         <v>322</v>
       </c>
+      <c r="L21">
+        <v>78</v>
+      </c>
       <c r="M21">
         <v>228</v>
       </c>
@@ -2208,6 +2211,9 @@
       <c r="R21">
         <v>34</v>
       </c>
+      <c r="T21">
+        <v>99</v>
+      </c>
       <c r="U21">
         <v>96</v>
       </c>
@@ -2217,6 +2223,9 @@
       <c r="W21">
         <v>31</v>
       </c>
+      <c r="Y21">
+        <v>651</v>
+      </c>
       <c r="Z21">
         <v>80</v>
       </c>
@@ -2224,8 +2233,8 @@
         <v>1363</v>
       </c>
       <c r="AB21" s="4">
-        <f>AB20+E21-E20+Z21-Z20+D21-D20+R21-R20+K21-K20+Q21-Q20+AA21-AA20+V21-V20+U21-U20+G21-G20+I21-I20+J21-J20+N21-N20+W21-W20+P21-P20+O21-O20+F21-F20+M21-M20+B21-B20</f>
-        <v>10771</v>
+        <f>SUM(B21:AA21)+X20+S20+H20+C20</f>
+        <v>10909</v>
       </c>
     </row>
   </sheetData>
@@ -2241,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2907,14 +2916,14 @@
         <v>21</v>
       </c>
       <c r="Y21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA21">
         <v>7</v>
       </c>
       <c r="AB21" s="4">
         <f>SUM(B21:AA21)</f>
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AG, AR, BE, SG, SH, SO, and ZG
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64F5F9B-361D-49FE-85A5-65A6B772F215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B6FA53-1576-4A7C-91B7-047D23375B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="1050" windowWidth="19470" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18015" yWindow="1365" windowWidth="19470" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,6 +2172,9 @@
       <c r="B21">
         <v>319</v>
       </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
       <c r="D21">
         <v>34</v>
       </c>
@@ -2214,6 +2217,9 @@
       <c r="R21">
         <v>34</v>
       </c>
+      <c r="S21">
+        <v>141</v>
+      </c>
       <c r="T21">
         <v>99</v>
       </c>
@@ -2236,8 +2242,35 @@
         <v>1363</v>
       </c>
       <c r="AB21" s="4">
-        <f>SUM(B21:AA21)+X20+S20+H20+C20</f>
-        <v>10909</v>
+        <f>SUM(B21:AA21)+X20+H20</f>
+        <v>10922</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B22">
+        <v>323</v>
+      </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>660</v>
+      </c>
+      <c r="Q22">
+        <v>280</v>
+      </c>
+      <c r="R22">
+        <v>35</v>
+      </c>
+      <c r="Z22">
+        <v>87</v>
+      </c>
+      <c r="AB22">
+        <f>SUM(B22:AA22)+AA21+Y21+X20+W21+V21+U21+T21+S21+P21+O21+N21+M21+L21+K21+J21+I21+H20+G21+F21+C21</f>
+        <v>11028</v>
       </c>
     </row>
   </sheetData>
@@ -2251,10 +2284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2927,6 +2960,66 @@
       <c r="AB21" s="4">
         <f>SUM(B21:AA21)</f>
         <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>15</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>60</v>
+      </c>
+      <c r="X22">
+        <v>21</v>
+      </c>
+      <c r="Y22">
+        <v>14</v>
+      </c>
+      <c r="AA22">
+        <v>7</v>
+      </c>
+      <c r="AB22" s="4">
+        <f>SUM(B22:AA22)</f>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated LU, BL, ZH
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E724F1B-C83F-492D-B506-AAA214B718D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08B3198-E78E-47D9-A5E2-27CDD0E6606F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="1335" windowWidth="17700" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="645" yWindow="1335" windowWidth="22065" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,16 +2257,16 @@
         <v>323</v>
       </c>
       <c r="D22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22">
         <v>660</v>
       </c>
       <c r="F22">
-        <v>368</v>
+        <v>422</v>
       </c>
       <c r="G22">
-        <v>569</v>
+        <v>505</v>
       </c>
       <c r="H22">
         <v>272</v>
@@ -2283,6 +2283,9 @@
       <c r="M22">
         <v>253</v>
       </c>
+      <c r="N22">
+        <v>271</v>
+      </c>
       <c r="Q22">
         <v>280</v>
       </c>
@@ -2298,9 +2301,12 @@
       <c r="Z22">
         <v>87</v>
       </c>
+      <c r="AA22">
+        <v>1476</v>
+      </c>
       <c r="AB22">
-        <f>SUM(B22:AA22)+AA21+Y21+X21+W21+T21+S21+P21+O21+N21+I21+C21</f>
-        <v>11473</v>
+        <f>SUM(B22:AA22)+Y21+X21+W21+T21+S21+P21+O21+I21+C21</f>
+        <v>11592</v>
       </c>
     </row>
   </sheetData>
@@ -2317,7 +2323,7 @@
   <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,6 +2762,9 @@
       <c r="K17">
         <v>3</v>
       </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
       <c r="N17">
         <v>2</v>
       </c>
@@ -2773,7 +2782,7 @@
       </c>
       <c r="AB17" s="4">
         <f t="shared" ref="AB17:AB22" si="0">SUM(B17:AA17)</f>
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -2804,6 +2813,9 @@
       <c r="K18">
         <v>5</v>
       </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
       <c r="N18">
         <v>2</v>
       </c>
@@ -2821,7 +2833,7 @@
       </c>
       <c r="AB18" s="4">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -2852,6 +2864,9 @@
       <c r="K19">
         <v>6</v>
       </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
       <c r="N19">
         <v>2</v>
       </c>
@@ -2872,7 +2887,7 @@
       </c>
       <c r="AB19" s="4">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -2903,6 +2918,9 @@
       <c r="K20">
         <v>6</v>
       </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
       <c r="N20">
         <v>2</v>
       </c>
@@ -2929,7 +2947,7 @@
       </c>
       <c r="AB20" s="4">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -2961,7 +2979,7 @@
         <v>6</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -2989,7 +3007,7 @@
       </c>
       <c r="AB21" s="4">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -3021,10 +3039,10 @@
         <v>9</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q22">
         <v>1</v>
@@ -3045,11 +3063,11 @@
         <v>14</v>
       </c>
       <c r="AA22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AB22" s="4">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AR and SH
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10645774-CF2A-48AB-9D92-0B537F07B8B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31628149-986A-4AF5-A57D-8EC3C328A5D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="855" windowWidth="22065" windowHeight="19665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA28" sqref="AA28"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,7 +2245,7 @@
         <v>31</v>
       </c>
       <c r="X21">
-        <v>2351</v>
+        <v>2215</v>
       </c>
       <c r="Y21">
         <v>651</v>
@@ -2258,7 +2258,7 @@
       </c>
       <c r="AB21" s="4">
         <f>SUM(B21:AA21)</f>
-        <v>11217</v>
+        <v>11081</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -2313,6 +2313,9 @@
       <c r="R22">
         <v>35</v>
       </c>
+      <c r="T22">
+        <v>99</v>
+      </c>
       <c r="U22">
         <v>110</v>
       </c>
@@ -2332,8 +2335,26 @@
         <v>1476</v>
       </c>
       <c r="AB22">
-        <f>SUM(B22:AA22)+X21+T21+S21+P21+C21</f>
-        <v>11897</v>
+        <f>SUM(B22:AA22)+X21+S21+P21+C21</f>
+        <v>11761</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43917</v>
+      </c>
+      <c r="D23">
+        <v>43</v>
+      </c>
+      <c r="R23">
+        <v>36</v>
+      </c>
+      <c r="Z23">
+        <v>94</v>
+      </c>
+      <c r="AB23">
+        <f>AB22+Z23-Z22+R23-R22+D23-D22</f>
+        <v>11770</v>
       </c>
     </row>
   </sheetData>
@@ -2347,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3072,7 +3093,7 @@
         <v>5</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S22">
         <v>1</v>
@@ -3097,7 +3118,70 @@
       </c>
       <c r="AB22" s="4">
         <f t="shared" si="0"/>
-        <v>193</v>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>21</v>
+      </c>
+      <c r="K23">
+        <v>9</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>67</v>
+      </c>
+      <c r="X23">
+        <v>21</v>
+      </c>
+      <c r="Y23">
+        <v>15</v>
+      </c>
+      <c r="AA23">
+        <v>9</v>
+      </c>
+      <c r="AB23" s="4">
+        <f t="shared" ref="AB23" si="1">SUM(B23:AA23)</f>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated and changed population density based on settlement area
</commit_message>
<xml_diff>
--- a/covid19_cases_switzerland.xlsx
+++ b/covid19_cases_switzerland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daenu\Code\covid19-cases-switzerland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C44B53-EBD2-4CCC-A94F-19C9F6F1E0D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10750DD-BC6B-42A3-B335-D1AC48689050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="855" windowWidth="22065" windowHeight="19665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="1140" windowWidth="15495" windowHeight="19680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_cases_switzerland" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Quellen" sheetId="4" r:id="rId3"/>
     <sheet name="Tests" sheetId="5" r:id="rId4"/>
     <sheet name="demographics" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="67">
   <si>
     <t>ZH</t>
   </si>
@@ -232,6 +233,12 @@
   </si>
   <si>
     <t>https://www.ge.ch/covid-19-professionnels-sante-reseau-soins</t>
+  </si>
+  <si>
+    <t>SettlementAreaHa</t>
+  </si>
+  <si>
+    <t>SettlementAreaKm2</t>
   </si>
 </sst>
 </file>
@@ -2373,7 +2380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7F9FF-DA82-4772-9651-CE094ADEC3E5}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
@@ -3621,7 +3628,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="G28" sqref="A1:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4792,4 +4799,940 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7A8D86-1045-4E12-8A88-5B033EF77DAB}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1520968</v>
+      </c>
+      <c r="C2">
+        <v>37796</v>
+      </c>
+      <c r="D2">
+        <f>C2*0.01</f>
+        <v>377.96</v>
+      </c>
+      <c r="E2">
+        <f>B2/D2</f>
+        <v>4024.150703778178</v>
+      </c>
+      <c r="F2">
+        <v>0.17</v>
+      </c>
+      <c r="G2">
+        <f>ROUND(B2*F2,0)</f>
+        <v>258565</v>
+      </c>
+      <c r="H2">
+        <v>4472</v>
+      </c>
+      <c r="I2">
+        <f>H2/B2</f>
+        <v>2.9402327991121442E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1034977</v>
+      </c>
+      <c r="C3">
+        <v>41197</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D27" si="0">C3*0.01</f>
+        <v>411.97</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E27" si="1">B3/D3</f>
+        <v>2512.2630288613245</v>
+      </c>
+      <c r="F3">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="G3">
+        <f>ROUND(B3*F3,0)</f>
+        <v>215275</v>
+      </c>
+      <c r="H3">
+        <v>3053</v>
+      </c>
+      <c r="I3">
+        <f>H3/B3</f>
+        <v>2.9498240057508522E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>799145</v>
+      </c>
+      <c r="C4">
+        <v>29940</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>299.40000000000003</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>2669.1549766199064</v>
+      </c>
+      <c r="F4">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G4">
+        <f>ROUND(B4*F4,0)</f>
+        <v>131060</v>
+      </c>
+      <c r="H4">
+        <v>2268</v>
+      </c>
+      <c r="I4">
+        <f>H4/B4</f>
+        <v>2.8380331479268468E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>678207</v>
+      </c>
+      <c r="C5">
+        <v>23854</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>238.54</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2843.1583801458878</v>
+      </c>
+      <c r="F5">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="G5">
+        <f>ROUND(B5*F5,0)</f>
+        <v>120043</v>
+      </c>
+      <c r="H5">
+        <v>1450</v>
+      </c>
+      <c r="I5">
+        <f>H5/B5</f>
+        <v>2.1379903185900469E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>507697</v>
+      </c>
+      <c r="C6">
+        <v>19408</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>194.08</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>2615.9161170651278</v>
+      </c>
+      <c r="F6">
+        <v>0.183</v>
+      </c>
+      <c r="G6">
+        <f>ROUND(B6*F6,0)</f>
+        <v>92909</v>
+      </c>
+      <c r="H6">
+        <v>1565</v>
+      </c>
+      <c r="I6">
+        <f>H6/B6</f>
+        <v>3.0825472673661654E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>495249</v>
+      </c>
+      <c r="C7">
+        <v>9416</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>94.16</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>5259.6537807986406</v>
+      </c>
+      <c r="F7">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G7">
+        <f>ROUND(B7*F7,0)</f>
+        <v>81221</v>
+      </c>
+      <c r="H7">
+        <v>1506</v>
+      </c>
+      <c r="I7">
+        <f>H7/B7</f>
+        <v>3.0408945803020301E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>409557</v>
+      </c>
+      <c r="C8">
+        <v>14384</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>143.84</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2847.3095105672969</v>
+      </c>
+      <c r="F8">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="G8">
+        <f>ROUND(B8*F8,0)</f>
+        <v>72082</v>
+      </c>
+      <c r="H8">
+        <v>977</v>
+      </c>
+      <c r="I8">
+        <f>H8/B8</f>
+        <v>2.3855043376135678E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>353343</v>
+      </c>
+      <c r="C9">
+        <v>15881</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>158.81</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2224.9417542975884</v>
+      </c>
+      <c r="F9">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G9">
+        <f>ROUND(B9*F9,0)</f>
+        <v>79856</v>
+      </c>
+      <c r="H9">
+        <v>1338</v>
+      </c>
+      <c r="I9">
+        <f>H9/B9</f>
+        <v>3.7866888547388798E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>343955</v>
+      </c>
+      <c r="C10">
+        <v>18463</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>184.63</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1862.9421004170504</v>
+      </c>
+      <c r="F10">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G10">
+        <f>ROUND(B10*F10,0)</f>
+        <v>67415</v>
+      </c>
+      <c r="H10">
+        <v>834</v>
+      </c>
+      <c r="I10">
+        <f>H10/B10</f>
+        <v>2.4247357939265312E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>318714</v>
+      </c>
+      <c r="C11">
+        <v>13998</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>139.97999999999999</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2276.8538362623235</v>
+      </c>
+      <c r="F11">
+        <v>0.157</v>
+      </c>
+      <c r="G11">
+        <f>ROUND(B11*F11,0)</f>
+        <v>50038</v>
+      </c>
+      <c r="H11">
+        <v>547</v>
+      </c>
+      <c r="I11">
+        <f>H11/B11</f>
+        <v>1.7162722691817743E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>288132</v>
+      </c>
+      <c r="C12">
+        <v>9025</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>90.25</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>3192.5983379501386</v>
+      </c>
+      <c r="F12">
+        <v>0.219</v>
+      </c>
+      <c r="G12">
+        <f>ROUND(B12*F12,0)</f>
+        <v>63101</v>
+      </c>
+      <c r="H12">
+        <v>582</v>
+      </c>
+      <c r="I12">
+        <f>H12/B12</f>
+        <v>2.0199075423764108E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>276472</v>
+      </c>
+      <c r="C13">
+        <v>12170</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>121.7</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>2271.7502054231718</v>
+      </c>
+      <c r="F13">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="G13">
+        <f>ROUND(B13*F13,0)</f>
+        <v>48659</v>
+      </c>
+      <c r="H13">
+        <v>570</v>
+      </c>
+      <c r="I13">
+        <f>H13/B13</f>
+        <v>2.0616915998726815E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>273194</v>
+      </c>
+      <c r="C14">
+        <v>10952</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>109.52</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>2494.4667640613588</v>
+      </c>
+      <c r="F14">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G14">
+        <f>ROUND(B14*F14,0)</f>
+        <v>53546</v>
+      </c>
+      <c r="H14">
+        <v>510</v>
+      </c>
+      <c r="I14">
+        <f>H14/B14</f>
+        <v>1.8668052739079189E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>198379</v>
+      </c>
+      <c r="C15">
+        <v>13863</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>138.63</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>1430.9961768736925</v>
+      </c>
+      <c r="F15">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="G15">
+        <f>ROUND(B15*F15,0)</f>
+        <v>42255</v>
+      </c>
+      <c r="H15">
+        <v>546</v>
+      </c>
+      <c r="I15">
+        <f>H15/B15</f>
+        <v>2.7523074518976303E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>194766</v>
+      </c>
+      <c r="C16">
+        <v>2628</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>26.28</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>7411.1872146118722</v>
+      </c>
+      <c r="F16">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="G16">
+        <f>ROUND(B16*F16,0)</f>
+        <v>38758</v>
+      </c>
+      <c r="H16">
+        <v>1199</v>
+      </c>
+      <c r="I16">
+        <f>H16/B16</f>
+        <v>6.1561052750480063E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>177964</v>
+      </c>
+      <c r="C17">
+        <v>6701</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>67.010000000000005</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>2655.7827189971645</v>
+      </c>
+      <c r="F17">
+        <v>0.19</v>
+      </c>
+      <c r="G17">
+        <f>ROUND(B17*F17,0)</f>
+        <v>33813</v>
+      </c>
+      <c r="H17">
+        <v>385</v>
+      </c>
+      <c r="I17">
+        <f>H17/B17</f>
+        <v>2.1633588815715538E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>159165</v>
+      </c>
+      <c r="C18">
+        <v>5499</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>54.99</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>2894.4353518821604</v>
+      </c>
+      <c r="F18">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="G18">
+        <f>ROUND(B18*F18,0)</f>
+        <v>28172</v>
+      </c>
+      <c r="H18">
+        <v>274</v>
+      </c>
+      <c r="I18">
+        <f>H18/B18</f>
+        <v>1.7214839945968021E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>126837</v>
+      </c>
+      <c r="C19">
+        <v>3306</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>33.06</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>3836.5698729582573</v>
+      </c>
+      <c r="F19">
+        <v>0.17</v>
+      </c>
+      <c r="G19">
+        <f>ROUND(B19*F19,0)</f>
+        <v>21562</v>
+      </c>
+      <c r="H19">
+        <v>206</v>
+      </c>
+      <c r="I19">
+        <f>H19/B19</f>
+        <v>1.6241317596600361E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>81991</v>
+      </c>
+      <c r="C20">
+        <v>3403</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>34.03</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>2409.3740816926243</v>
+      </c>
+      <c r="F20">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="G20">
+        <f>ROUND(B20*F20,0)</f>
+        <v>17382</v>
+      </c>
+      <c r="H20">
+        <v>186</v>
+      </c>
+      <c r="I20">
+        <f>H20/B20</f>
+        <v>2.2685416692075958E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>73419</v>
+      </c>
+      <c r="C21">
+        <v>5615</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>56.15</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>1307.5512021371328</v>
+      </c>
+      <c r="F21">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="G21">
+        <f>ROUND(B21*F21,0)</f>
+        <v>15345</v>
+      </c>
+      <c r="H21">
+        <v>145</v>
+      </c>
+      <c r="I21">
+        <f>H21/B21</f>
+        <v>1.9749656083575097E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>55234</v>
+      </c>
+      <c r="C22">
+        <v>2231</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>22.31</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>2475.7507844016136</v>
+      </c>
+      <c r="F22">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="G22">
+        <f>ROUND(B22*F22,0)</f>
+        <v>10881</v>
+      </c>
+      <c r="H22">
+        <v>208</v>
+      </c>
+      <c r="I22">
+        <f>H22/B22</f>
+        <v>3.7657964297353082E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>43223</v>
+      </c>
+      <c r="C23">
+        <v>1481</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>14.81</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>2918.5010128291692</v>
+      </c>
+      <c r="F23">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="G23">
+        <f>ROUND(B23*F23,0)</f>
+        <v>8774</v>
+      </c>
+      <c r="H23">
+        <v>73</v>
+      </c>
+      <c r="I23">
+        <f>H23/B23</f>
+        <v>1.6889156236263101E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>40403</v>
+      </c>
+      <c r="C24">
+        <v>1995</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>19.95</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>2025.2130325814537</v>
+      </c>
+      <c r="F24">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="G24">
+        <f>ROUND(B24*F24,0)</f>
+        <v>8121</v>
+      </c>
+      <c r="H24">
+        <v>86</v>
+      </c>
+      <c r="I24">
+        <f>H24/B24</f>
+        <v>2.1285548102863649E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>37841</v>
+      </c>
+      <c r="C25">
+        <v>1879</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>18.79</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>2013.8903672166048</v>
+      </c>
+      <c r="F25">
+        <v>0.188</v>
+      </c>
+      <c r="G25">
+        <f>ROUND(B25*F25,0)</f>
+        <v>7114</v>
+      </c>
+      <c r="H25">
+        <v>50</v>
+      </c>
+      <c r="I25">
+        <f>H25/B25</f>
+        <v>1.3213181469834306E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>36433</v>
+      </c>
+      <c r="C26">
+        <v>2000</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1821.65</v>
+      </c>
+      <c r="F26">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="G26">
+        <f>ROUND(B26*F26,0)</f>
+        <v>7432</v>
+      </c>
+      <c r="H26">
+        <v>63</v>
+      </c>
+      <c r="I26">
+        <f>H26/B26</f>
+        <v>1.7292015480471002E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>16145</v>
+      </c>
+      <c r="C27">
+        <v>813</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>1985.8548585485853</v>
+      </c>
+      <c r="F27">
+        <v>0.191</v>
+      </c>
+      <c r="G27">
+        <f>ROUND(B27*F27,0)</f>
+        <v>3084</v>
+      </c>
+      <c r="H27">
+        <v>18</v>
+      </c>
+      <c r="I27">
+        <f>H27/B27</f>
+        <v>1.1148962527098173E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>SUM(B2:B27)</f>
+        <v>8541410</v>
+      </c>
+      <c r="E28">
+        <f>AVERAGE(E2:E27)</f>
+        <v>2780.0736988837816</v>
+      </c>
+      <c r="F28">
+        <f>AVERAGE(F2:F27)</f>
+        <v>0.19099999999999998</v>
+      </c>
+      <c r="G28">
+        <f>SUM(G2:G27)</f>
+        <v>1576463</v>
+      </c>
+      <c r="H28">
+        <f>SUM(H2:H27)</f>
+        <v>23111</v>
+      </c>
+      <c r="I28">
+        <f>H28/B28</f>
+        <v>2.7057593535493554E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>